<commit_message>
finished background and added capstone prior work
</commit_message>
<xml_diff>
--- a/Thesis Charts and Graphs.xlsx
+++ b/Thesis Charts and Graphs.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://buckeyemailosu.sharepoint.com/sites/Tumortrackingresearch/Shared Documents/General/Theses/Isaac/Master's Thesis/ohio-state-coe-dissertation-template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{9ADA1457-FD2B-CE4C-A959-04A3C32A4882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AE940E13-1D07-F248-B825-69C03399F77F}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="8_{9ADA1457-FD2B-CE4C-A959-04A3C32A4882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{11CFF670-2FEA-5A45-A737-4B77696163E2}"/>
   <bookViews>
-    <workbookView xWindow="980" yWindow="500" windowWidth="34860" windowHeight="21900" xr2:uid="{16E6A821-3DC4-194B-96AE-E7BDD0CEA9F6}"/>
+    <workbookView xWindow="980" yWindow="500" windowWidth="34860" windowHeight="21900" activeTab="1" xr2:uid="{16E6A821-3DC4-194B-96AE-E7BDD0CEA9F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Literature Review" sheetId="1" r:id="rId1"/>
+    <sheet name="Introduction" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Seroma Visibility (RefID 25)</t>
   </si>
@@ -52,12 +53,61 @@
   <si>
     <t>Not Visible</t>
   </si>
+  <si>
+    <t>Team/Researcher</t>
+  </si>
+  <si>
+    <t>General Contribution(s)</t>
+  </si>
+  <si>
+    <t>Time Working on Project</t>
+  </si>
+  <si>
+    <t>Senior Capstone Group</t>
+  </si>
+  <si>
+    <t>- Identified initial pain points and opportunity
+- Evaluated various end-product concepts
+- Selected ideal form factor and developed initial device prototype</t>
+  </si>
+  <si>
+    <t>2022</t>
+  </si>
+  <si>
+    <t>Adrian Bakhtar</t>
+  </si>
+  <si>
+    <t>- Continued work started by senior capstone team
+- Worked with stakeholders to refine device design
+- Optimized device geometry, printability, and adhesive capabilities
+- Defended master's thesis and is continuing research through a PhD</t>
+  </si>
+  <si>
+    <t>2022 – Present</t>
+  </si>
+  <si>
+    <t>Zuhaib Jama</t>
+  </si>
+  <si>
+    <t>- Evaluated potential stresses experienced by the device via FEM
+- Presented findings at research poster symposium</t>
+  </si>
+  <si>
+    <t>Isaac Einstein</t>
+  </si>
+  <si>
+    <t>- Evaluated material properties of device base material
+- Presented findings through a research poster symposium and undergraduate thesis</t>
+  </si>
+  <si>
+    <t>2023 - 2024</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -70,6 +120,13 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -93,7 +150,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -286,11 +343,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -310,6 +397,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1607,7 +1709,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDAF9E8A-4B25-1B41-82F3-06803E42F3DE}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="173" workbookViewId="0">
+    <sheetView zoomScale="173" workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
@@ -1705,13 +1807,101 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF6216C1-5646-664A-92BE-4FE78C39E120}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="173" workbookViewId="0">
+      <selection activeCell="C2" sqref="A1:C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="18.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="9"/>
+    </row>
+    <row r="2" spans="1:4" ht="112" x14ac:dyDescent="0.2">
+      <c r="A2" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="10"/>
+    </row>
+    <row r="3" spans="1:4" ht="208" x14ac:dyDescent="0.2">
+      <c r="A3" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="10"/>
+    </row>
+    <row r="4" spans="1:4" ht="96" x14ac:dyDescent="0.2">
+      <c r="A4" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="17">
+        <v>2024</v>
+      </c>
+      <c r="D4" s="10"/>
+    </row>
+    <row r="5" spans="1:4" ht="112" x14ac:dyDescent="0.2">
+      <c r="A5" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="10"/>
+    </row>
+    <row r="6" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="12"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="14"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="40c2d214-4ca5-4604-be72-e6c4439e5276">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="581c75f3-c23e-4d61-ac2d-458e1df0a137" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1922,20 +2112,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="40c2d214-4ca5-4604-be72-e6c4439e5276">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="581c75f3-c23e-4d61-ac2d-458e1df0a137" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77CBFA7D-3A0A-48A4-8B12-895234E5D6E5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F17E70AE-5CD9-46AD-9CD7-253B7D5337F5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="40c2d214-4ca5-4604-be72-e6c4439e5276"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="581c75f3-c23e-4d61-ac2d-458e1df0a137"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1960,18 +2157,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F17E70AE-5CD9-46AD-9CD7-253B7D5337F5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77CBFA7D-3A0A-48A4-8B12-895234E5D6E5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="40c2d214-4ca5-4604-be72-e6c4439e5276"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="581c75f3-c23e-4d61-ac2d-458e1df0a137"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Finished capstone prior work
</commit_message>
<xml_diff>
--- a/Thesis Charts and Graphs.xlsx
+++ b/Thesis Charts and Graphs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://buckeyemailosu.sharepoint.com/sites/Tumortrackingresearch/Shared Documents/General/Theses/Isaac/Master's Thesis/ohio-state-coe-dissertation-template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="8_{9ADA1457-FD2B-CE4C-A959-04A3C32A4882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{11CFF670-2FEA-5A45-A737-4B77696163E2}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="8_{9ADA1457-FD2B-CE4C-A959-04A3C32A4882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4DAB7EC6-AE8B-EC46-9CE9-418AC874587F}"/>
   <bookViews>
     <workbookView xWindow="980" yWindow="500" windowWidth="34860" windowHeight="21900" activeTab="1" xr2:uid="{16E6A821-3DC4-194B-96AE-E7BDD0CEA9F6}"/>
   </bookViews>
@@ -123,7 +123,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="7"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -150,7 +150,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -344,40 +344,21 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
+      <right/>
+      <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -399,19 +380,31 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1812,72 +1805,74 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="173" workbookViewId="0">
-      <selection activeCell="C2" sqref="A1:C5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="18.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.83203125" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="20" t="s">
         <v>7</v>
       </c>
       <c r="D1" s="9"/>
     </row>
-    <row r="2" spans="1:4" ht="112" x14ac:dyDescent="0.2">
-      <c r="A2" s="20" t="s">
+    <row r="2" spans="1:4" ht="67" x14ac:dyDescent="0.2">
+      <c r="A2" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="22" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="10"/>
     </row>
-    <row r="3" spans="1:4" ht="208" x14ac:dyDescent="0.2">
-      <c r="A3" s="20" t="s">
+    <row r="3" spans="1:4" ht="89" x14ac:dyDescent="0.2">
+      <c r="A3" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="22" t="s">
         <v>13</v>
       </c>
       <c r="D3" s="10"/>
     </row>
-    <row r="4" spans="1:4" ht="96" x14ac:dyDescent="0.2">
-      <c r="A4" s="20" t="s">
+    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+      <c r="A4" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="17">
+      <c r="C4" s="22">
         <v>2024</v>
       </c>
       <c r="D4" s="10"/>
     </row>
-    <row r="5" spans="1:4" ht="112" x14ac:dyDescent="0.2">
-      <c r="A5" s="20" t="s">
+    <row r="5" spans="1:4" ht="57" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="25" t="s">
         <v>18</v>
       </c>
       <c r="D5" s="10"/>
@@ -1905,8 +1900,8 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010020A0C45D55D81B409E1ED58F2E9DADA4" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="174658b08774cdecd53c756c6c7cbca5">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="40c2d214-4ca5-4604-be72-e6c4439e5276" xmlns:ns3="581c75f3-c23e-4d61-ac2d-458e1df0a137" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c9bb98d4c33526278c218015f2341df8" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010020A0C45D55D81B409E1ED58F2E9DADA4" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4fa2050de8fd1970c7139c0348e41ca3">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="40c2d214-4ca5-4604-be72-e6c4439e5276" xmlns:ns3="581c75f3-c23e-4d61-ac2d-458e1df0a137" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f9a6f9f6c893a0ba7e28c007d9267f0e" ns2:_="" ns3:_="">
     <xsd:import namespace="40c2d214-4ca5-4604-be72-e6c4439e5276"/>
     <xsd:import namespace="581c75f3-c23e-4d61-ac2d-458e1df0a137"/>
     <xsd:element name="properties">
@@ -2138,22 +2133,7 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BEBCE389-149B-4470-9475-120118DED985}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="40c2d214-4ca5-4604-be72-e6c4439e5276"/>
-    <ds:schemaRef ds:uri="581c75f3-c23e-4d61-ac2d-458e1df0a137"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDAD4442-CD32-4282-A934-0FFE683B5B87}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
Finished current methods of lit review
</commit_message>
<xml_diff>
--- a/Thesis Charts and Graphs.xlsx
+++ b/Thesis Charts and Graphs.xlsx
@@ -8,14 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://buckeyemailosu.sharepoint.com/sites/Tumortrackingresearch/Shared Documents/General/Theses/Isaac/Master's Thesis/ohio-state-coe-dissertation-template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="8_{9ADA1457-FD2B-CE4C-A959-04A3C32A4882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4DAB7EC6-AE8B-EC46-9CE9-418AC874587F}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="8_{9ADA1457-FD2B-CE4C-A959-04A3C32A4882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F3169B6-48DE-F44D-8094-79760563A7A8}"/>
   <bookViews>
     <workbookView xWindow="980" yWindow="500" windowWidth="34860" windowHeight="21900" activeTab="1" xr2:uid="{16E6A821-3DC4-194B-96AE-E7BDD0CEA9F6}"/>
   </bookViews>
   <sheets>
-    <sheet name="Literature Review" sheetId="1" r:id="rId1"/>
-    <sheet name="Introduction" sheetId="2" r:id="rId2"/>
+    <sheet name="Introduction" sheetId="2" r:id="rId1"/>
+    <sheet name="Literature Review" sheetId="1" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">'Literature Review'!$A$2:$A$5</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'Literature Review'!$B$2:$B$5</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'Literature Review'!$A$2:$A$5</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'Literature Review'!$B$2:$B$5</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -374,13 +380,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -405,6 +405,12 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -501,13 +507,28 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:pieChart>
-        <c:varyColors val="1"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln w="19050">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:dPt>
             <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
@@ -528,6 +549,7 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
@@ -551,6 +573,7 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
@@ -574,6 +597,7 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
@@ -630,23 +654,25 @@
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="1"/>
-            <c:leaderLines>
-              <c:spPr>
-                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="35000"/>
-                      <a:lumOff val="65000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:round/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:leaderLines>
+            <c:showLeaderLines val="0"/>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -703,10 +729,116 @@
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
-          <c:showLeaderLines val="1"/>
         </c:dLbls>
-        <c:firstSliceAng val="0"/>
-      </c:pieChart>
+        <c:gapWidth val="100"/>
+        <c:axId val="2142970144"/>
+        <c:axId val="2142998880"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2142970144"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2142998880"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2142998880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2142970144"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1699,11 +1831,99 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF6216C1-5646-664A-92BE-4FE78C39E120}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView zoomScale="173" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.83203125" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="9"/>
+    </row>
+    <row r="2" spans="1:4" ht="67" x14ac:dyDescent="0.2">
+      <c r="A2" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="10"/>
+    </row>
+    <row r="3" spans="1:4" ht="89" x14ac:dyDescent="0.2">
+      <c r="A3" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="10"/>
+    </row>
+    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+      <c r="A4" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="20">
+        <v>2024</v>
+      </c>
+      <c r="D4" s="10"/>
+    </row>
+    <row r="5" spans="1:4" ht="57" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="10"/>
+    </row>
+    <row r="6" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="12"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="14"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDAF9E8A-4B25-1B41-82F3-06803E42F3DE}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView zoomScale="173" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" zoomScale="173" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1714,10 +1934,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
+      <c r="B1" s="25"/>
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
       <c r="E1" s="8"/>
@@ -1800,103 +2020,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF6216C1-5646-664A-92BE-4FE78C39E120}">
-  <dimension ref="A1:D6"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="173" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="2.83203125" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="9"/>
-    </row>
-    <row r="2" spans="1:4" ht="67" x14ac:dyDescent="0.2">
-      <c r="A2" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="10"/>
-    </row>
-    <row r="3" spans="1:4" ht="89" x14ac:dyDescent="0.2">
-      <c r="A3" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="10"/>
-    </row>
-    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.2">
-      <c r="A4" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="22">
-        <v>2024</v>
-      </c>
-      <c r="D4" s="10"/>
-    </row>
-    <row r="5" spans="1:4" ht="57" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="10"/>
-    </row>
-    <row r="6" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="14"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="40c2d214-4ca5-4604-be72-e6c4439e5276">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="581c75f3-c23e-4d61-ac2d-458e1df0a137" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2107,39 +2237,56 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="40c2d214-4ca5-4604-be72-e6c4439e5276">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="581c75f3-c23e-4d61-ac2d-458e1df0a137" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F17E70AE-5CD9-46AD-9CD7-253B7D5337F5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77CBFA7D-3A0A-48A4-8B12-895234E5D6E5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="40c2d214-4ca5-4604-be72-e6c4439e5276"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="581c75f3-c23e-4d61-ac2d-458e1df0a137"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDAD4442-CD32-4282-A934-0FFE683B5B87}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDAD4442-CD32-4282-A934-0FFE683B5B87}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="40c2d214-4ca5-4604-be72-e6c4439e5276"/>
+    <ds:schemaRef ds:uri="581c75f3-c23e-4d61-ac2d-458e1df0a137"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77CBFA7D-3A0A-48A4-8B12-895234E5D6E5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F17E70AE-5CD9-46AD-9CD7-253B7D5337F5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="581c75f3-c23e-4d61-ac2d-458e1df0a137"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="40c2d214-4ca5-4604-be72-e6c4439e5276"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Finished 3D printing section of literature review
</commit_message>
<xml_diff>
--- a/Thesis Charts and Graphs.xlsx
+++ b/Thesis Charts and Graphs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://buckeyemailosu.sharepoint.com/sites/Tumortrackingresearch/Shared Documents/General/Theses/Isaac/Master's Thesis/ohio-state-coe-dissertation-template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="8_{9ADA1457-FD2B-CE4C-A959-04A3C32A4882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F3169B6-48DE-F44D-8094-79760563A7A8}"/>
+  <xr:revisionPtr revIDLastSave="71" documentId="8_{9ADA1457-FD2B-CE4C-A959-04A3C32A4882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{54293F79-F7D0-AE41-A5A0-9E330DB5AB5D}"/>
   <bookViews>
     <workbookView xWindow="980" yWindow="500" windowWidth="34860" windowHeight="21900" activeTab="1" xr2:uid="{16E6A821-3DC4-194B-96AE-E7BDD0CEA9F6}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Seroma Visibility (RefID 25)</t>
   </si>
@@ -107,6 +107,51 @@
   </si>
   <si>
     <t>2023 - 2024</t>
+  </si>
+  <si>
+    <t>Material</t>
+  </si>
+  <si>
+    <t>Extrusion Temperature (ºC)</t>
+  </si>
+  <si>
+    <t>Bed Temperature (ºC)</t>
+  </si>
+  <si>
+    <t>Glass Transition Temperature (ºC)</t>
+  </si>
+  <si>
+    <t>160 – 230</t>
+  </si>
+  <si>
+    <t>20 – 60</t>
+  </si>
+  <si>
+    <t>60 – 65</t>
+  </si>
+  <si>
+    <t>115 – 145</t>
+  </si>
+  <si>
+    <t>PCL (RefID 418)</t>
+  </si>
+  <si>
+    <t>PLA (RefID 307)</t>
+  </si>
+  <si>
+    <t>30 – 45</t>
+  </si>
+  <si>
+    <t>35 – 40</t>
+  </si>
+  <si>
+    <t>PLCL (RefID 18, 204)</t>
+  </si>
+  <si>
+    <t>180 – 230</t>
+  </si>
+  <si>
+    <t>18 – 30</t>
   </si>
 </sst>
 </file>
@@ -156,7 +201,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -360,11 +405,56 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -413,6 +503,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1920,17 +2018,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDAF9E8A-4B25-1B41-82F3-06803E42F3DE}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="173" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A13" sqref="A13:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="13.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -2010,6 +2110,80 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
       <c r="H11" s="14"/>
+    </row>
+    <row r="12" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="26"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="9"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="10"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="10"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="5">
+        <v>-60</v>
+      </c>
+      <c r="E15" s="10"/>
+    </row>
+    <row r="16" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" s="10"/>
+    </row>
+    <row r="17" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="12"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Revised 3D printing section of lit review
</commit_message>
<xml_diff>
--- a/Thesis Charts and Graphs.xlsx
+++ b/Thesis Charts and Graphs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://buckeyemailosu.sharepoint.com/sites/Tumortrackingresearch/Shared Documents/General/Theses/Isaac/Master's Thesis/ohio-state-coe-dissertation-template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="71" documentId="8_{9ADA1457-FD2B-CE4C-A959-04A3C32A4882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{54293F79-F7D0-AE41-A5A0-9E330DB5AB5D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{BDDE5BD9-9B9B-1147-BD62-444B36ECC1DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="980" yWindow="500" windowWidth="34860" windowHeight="21900" activeTab="1" xr2:uid="{16E6A821-3DC4-194B-96AE-E7BDD0CEA9F6}"/>
   </bookViews>
@@ -2021,7 +2021,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="173" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:D16"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Working on material properties of lit review
</commit_message>
<xml_diff>
--- a/Thesis Charts and Graphs.xlsx
+++ b/Thesis Charts and Graphs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://buckeyemailosu.sharepoint.com/sites/Tumortrackingresearch/Shared Documents/General/Theses/Isaac/Master's Thesis/ohio-state-coe-dissertation-template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{BDDE5BD9-9B9B-1147-BD62-444B36ECC1DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="14_{BDDE5BD9-9B9B-1147-BD62-444B36ECC1DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6112CF1B-D4B9-4648-A88E-0102AB67B72A}"/>
   <bookViews>
     <workbookView xWindow="980" yWindow="500" windowWidth="34860" windowHeight="21900" activeTab="1" xr2:uid="{16E6A821-3DC4-194B-96AE-E7BDD0CEA9F6}"/>
   </bookViews>
@@ -16,12 +16,6 @@
     <sheet name="Introduction" sheetId="2" r:id="rId1"/>
     <sheet name="Literature Review" sheetId="1" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'Literature Review'!$A$2:$A$5</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'Literature Review'!$B$2:$B$5</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'Literature Review'!$A$2:$A$5</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'Literature Review'!$B$2:$B$5</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -43,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
   <si>
     <t>Seroma Visibility (RefID 25)</t>
   </si>
@@ -152,6 +146,59 @@
   </si>
   <si>
     <t>18 – 30</t>
+  </si>
+  <si>
+    <t>PCL</t>
+  </si>
+  <si>
+    <t>Tensile Modulus (Et)</t>
+  </si>
+  <si>
+    <t>Compressive Modulus (Ecomp)</t>
+  </si>
+  <si>
+    <t>Tensile Yield Strength</t>
+  </si>
+  <si>
+    <t>440 ± 3 Mpa (ID46)
+417 ± 25 Mpa (ID133)</t>
+  </si>
+  <si>
+    <t>455 ± 2 Mpa (ID46)</t>
+  </si>
+  <si>
+    <t>414 ± 10 Mpa (ID46)</t>
+  </si>
+  <si>
+    <t>17.82 ± 0.47 Mpa (ID46)
+14.7 ± 1.3 MPa (ID133)</t>
+  </si>
+  <si>
+    <t>PLA</t>
+  </si>
+  <si>
+    <t>PLCL (70/30)</t>
+  </si>
+  <si>
+    <t>12 ± 1.2 Mpa (Secant Modulus at 0.2% strain) (ID31)</t>
+  </si>
+  <si>
+    <t>17.2 ± 0.7 MPa (ID31)
+16.1 ± 3.2 Mpa (ID19)</t>
+  </si>
+  <si>
+    <t>55.9 ± 6.5 (ID133)
+50 Mpa (ID434)</t>
+  </si>
+  <si>
+    <t>Flexural Modulus (Eflex)</t>
+  </si>
+  <si>
+    <t>3800 Mpa (ID343)</t>
+  </si>
+  <si>
+    <t>3015 ± 86 Mpa (ID133)
+3600 Mpa (ID343)</t>
   </si>
 </sst>
 </file>
@@ -454,7 +501,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -497,12 +544,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
@@ -511,6 +552,18 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -877,6 +930,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="2142998880"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -935,6 +989,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="2142970144"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
@@ -2018,26 +2073,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDAF9E8A-4B25-1B41-82F3-06803E42F3DE}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="173" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="173" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25"/>
+      <c r="B1" s="33"/>
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
       <c r="E1" s="8"/>
@@ -2112,35 +2168,35 @@
       <c r="H11" s="14"/>
     </row>
     <row r="12" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="26"/>
+      <c r="A12" s="24"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
       <c r="E12" s="9"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="29" t="s">
+      <c r="A13" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="30" t="s">
+      <c r="C13" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="31" t="s">
+      <c r="D13" s="29" t="s">
         <v>22</v>
       </c>
       <c r="E13" s="10"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="32" t="s">
+      <c r="A14" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="27" t="s">
+      <c r="C14" s="25" t="s">
         <v>24</v>
       </c>
       <c r="D14" s="5" t="s">
@@ -2149,13 +2205,13 @@
       <c r="E14" s="10"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="32" t="s">
+      <c r="A15" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="27" t="s">
+      <c r="B15" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="27" t="s">
+      <c r="C15" s="25" t="s">
         <v>29</v>
       </c>
       <c r="D15" s="5">
@@ -2164,13 +2220,13 @@
       <c r="E15" s="10"/>
     </row>
     <row r="16" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="28" t="s">
+      <c r="B16" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="28" t="s">
+      <c r="C16" s="26" t="s">
         <v>33</v>
       </c>
       <c r="D16" s="7" t="s">
@@ -2184,6 +2240,68 @@
       <c r="C17" s="13"/>
       <c r="D17" s="13"/>
       <c r="E17" s="14"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="E19" s="34" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A20" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="E20" s="35" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A21" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" s="34"/>
+      <c r="D21" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" s="35" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A22" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="34"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="35" t="s">
+        <v>45</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2204,6 +2322,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="40c2d214-4ca5-4604-be72-e6c4439e5276">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="581c75f3-c23e-4d61-ac2d-458e1df0a137" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010020A0C45D55D81B409E1ED58F2E9DADA4" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4fa2050de8fd1970c7139c0348e41ca3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="40c2d214-4ca5-4604-be72-e6c4439e5276" xmlns:ns3="581c75f3-c23e-4d61-ac2d-458e1df0a137" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f9a6f9f6c893a0ba7e28c007d9267f0e" ns2:_="" ns3:_="">
     <xsd:import namespace="40c2d214-4ca5-4604-be72-e6c4439e5276"/>
@@ -2410,17 +2539,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="40c2d214-4ca5-4604-be72-e6c4439e5276">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="581c75f3-c23e-4d61-ac2d-458e1df0a137" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77CBFA7D-3A0A-48A4-8B12-895234E5D6E5}">
   <ds:schemaRefs>
@@ -2430,6 +2548,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F17E70AE-5CD9-46AD-9CD7-253B7D5337F5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="581c75f3-c23e-4d61-ac2d-458e1df0a137"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="40c2d214-4ca5-4604-be72-e6c4439e5276"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDAD4442-CD32-4282-A934-0FFE683B5B87}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2446,21 +2581,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F17E70AE-5CD9-46AD-9CD7-253B7D5337F5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="581c75f3-c23e-4d61-ac2d-458e1df0a137"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="40c2d214-4ca5-4604-be72-e6c4439e5276"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
working on mechanical testing section of lit review
</commit_message>
<xml_diff>
--- a/Thesis Charts and Graphs.xlsx
+++ b/Thesis Charts and Graphs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://buckeyemailosu.sharepoint.com/sites/Tumortrackingresearch/Shared Documents/General/Theses/Isaac/Master's Thesis/ohio-state-coe-dissertation-template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="35" documentId="14_{BDDE5BD9-9B9B-1147-BD62-444B36ECC1DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6112CF1B-D4B9-4648-A88E-0102AB67B72A}"/>
+  <xr:revisionPtr revIDLastSave="79" documentId="14_{BDDE5BD9-9B9B-1147-BD62-444B36ECC1DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E397CCAE-AE1B-464C-8EA5-F80EF5A09893}"/>
   <bookViews>
     <workbookView xWindow="980" yWindow="500" windowWidth="34860" windowHeight="21900" activeTab="1" xr2:uid="{16E6A821-3DC4-194B-96AE-E7BDD0CEA9F6}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="75">
   <si>
     <t>Seroma Visibility (RefID 25)</t>
   </si>
@@ -199,6 +199,81 @@
   <si>
     <t>3015 ± 86 Mpa (ID133)
 3600 Mpa (ID343)</t>
+  </si>
+  <si>
+    <t>Strength</t>
+  </si>
+  <si>
+    <t>Ability of a material to resist externally applied forces without breaking or yielding</t>
+  </si>
+  <si>
+    <t>Stiffness</t>
+  </si>
+  <si>
+    <t>Ability of a material to resist deformation under stress</t>
+  </si>
+  <si>
+    <t>Elasticity</t>
+  </si>
+  <si>
+    <t>Ability of a material to regain its orginial shape after deformation</t>
+  </si>
+  <si>
+    <t>Plasticity</t>
+  </si>
+  <si>
+    <t>Ability of a material to undergo some degree of permanent deformation without failure</t>
+  </si>
+  <si>
+    <t>Brittleness</t>
+  </si>
+  <si>
+    <t>Ability of a material to fracture or break with minimal elongation</t>
+  </si>
+  <si>
+    <t>Term</t>
+  </si>
+  <si>
+    <t>Definition</t>
+  </si>
+  <si>
+    <t>Standard</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>ASTM D5947-24</t>
+  </si>
+  <si>
+    <t>Standard Test Methods for Physical Dimensions of Solid Plastics Specimens</t>
+  </si>
+  <si>
+    <t>RefID</t>
+  </si>
+  <si>
+    <t>ASTM F640-20</t>
+  </si>
+  <si>
+    <t>Standard Test Methods for Determining Radiopacity for Medical Use</t>
+  </si>
+  <si>
+    <t>ASTM D1238-23a</t>
+  </si>
+  <si>
+    <t>Standard Test Metod for Melt Flow Rates of Thermopastics by Extrusion Plastometer</t>
+  </si>
+  <si>
+    <t>ASTM D790-17</t>
+  </si>
+  <si>
+    <t>Standard Test Methods for Flexural Properties of Unreinforced and Reinforced Plastics and Electrical Insulation Materials</t>
+  </si>
+  <si>
+    <t>ASTM D638-14</t>
+  </si>
+  <si>
+    <t>Standard Test Method for Tensile Properties of Plastics</t>
   </si>
 </sst>
 </file>
@@ -501,7 +576,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -544,7 +619,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -563,6 +637,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2073,91 +2157,208 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDAF9E8A-4B25-1B41-82F3-06803E42F3DE}">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="173" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="173" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11:K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="1"/>
+    <col min="6" max="9" width="10.83203125" style="1"/>
+    <col min="10" max="10" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="70.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33"/>
+      <c r="B1" s="32"/>
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
       <c r="E1" s="8"/>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
       <c r="H1" s="9"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" s="8"/>
+      <c r="J1" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="K1" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="L1" s="9"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="3">
         <v>8</v>
       </c>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
       <c r="H2" s="10"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I2" s="35"/>
+      <c r="J2" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="L2" s="10"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="5">
         <v>10</v>
       </c>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
       <c r="H3" s="10"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I3" s="35"/>
+      <c r="J3" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="L3" s="10"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="5">
         <v>6</v>
       </c>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
       <c r="H4" s="10"/>
-    </row>
-    <row r="5" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I4" s="35"/>
+      <c r="J4" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="L4" s="10"/>
+    </row>
+    <row r="5" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="7">
         <v>6</v>
       </c>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
       <c r="H5" s="10"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I5" s="35"/>
+      <c r="J5" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="L5" s="10"/>
+    </row>
+    <row r="6" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
       <c r="H6" s="10"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I6" s="35"/>
+      <c r="J6" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="L6" s="10"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="11"/>
+      <c r="B7" s="35"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
       <c r="H7" s="10"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I7" s="35"/>
+      <c r="J7" s="35"/>
+      <c r="K7" s="35"/>
+      <c r="L7" s="10"/>
+    </row>
+    <row r="8" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
       <c r="H8" s="10"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I8" s="35"/>
+      <c r="J8" s="35"/>
+      <c r="K8" s="35"/>
+      <c r="L8" s="10"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="11"/>
+      <c r="B9" s="35"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="35"/>
       <c r="H9" s="10"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="9"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="11"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="35"/>
       <c r="H10" s="10"/>
-    </row>
-    <row r="11" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I10" s="35"/>
+      <c r="J10" s="35"/>
+      <c r="K10" s="35"/>
+      <c r="L10" s="10"/>
+    </row>
+    <row r="11" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
       <c r="B11" s="13"/>
       <c r="C11" s="13"/>
@@ -2166,142 +2367,252 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
       <c r="H11" s="14"/>
-    </row>
-    <row r="12" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="24"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="9"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="27" t="s">
+      <c r="I11" s="35"/>
+      <c r="J11" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="K11" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="L11" s="10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="11"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="35"/>
+      <c r="I12" s="35"/>
+      <c r="J12" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="K12" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="L12" s="10">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="28" t="s">
+      <c r="C13" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="29" t="s">
+      <c r="D13" s="28" t="s">
         <v>22</v>
       </c>
       <c r="E13" s="10"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="30" t="s">
+      <c r="F13" s="35"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="35"/>
+      <c r="I13" s="35"/>
+      <c r="J13" s="35" t="s">
+        <v>67</v>
+      </c>
+      <c r="K13" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="L13" s="10">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="25" t="s">
+      <c r="B14" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="25" t="s">
+      <c r="C14" s="24" t="s">
         <v>24</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>25</v>
       </c>
       <c r="E14" s="10"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="30" t="s">
+      <c r="F14" s="35"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="35"/>
+      <c r="I14" s="35"/>
+      <c r="J14" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="K14" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="L14" s="10">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="25" t="s">
+      <c r="B15" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="25" t="s">
+      <c r="C15" s="24" t="s">
         <v>29</v>
       </c>
       <c r="D15" s="5">
         <v>-60</v>
       </c>
       <c r="E15" s="10"/>
-    </row>
-    <row r="16" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="31" t="s">
+      <c r="F15" s="35"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="35"/>
+      <c r="I15" s="35"/>
+      <c r="J15" s="35" t="s">
+        <v>71</v>
+      </c>
+      <c r="K15" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="L15" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="26" t="s">
+      <c r="B16" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="26" t="s">
+      <c r="C16" s="25" t="s">
         <v>33</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>30</v>
       </c>
       <c r="E16" s="10"/>
-    </row>
-    <row r="17" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F16" s="35"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35" t="s">
+        <v>73</v>
+      </c>
+      <c r="K16" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="L16" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12"/>
       <c r="B17" s="13"/>
       <c r="C17" s="13"/>
       <c r="D17" s="13"/>
       <c r="E17" s="14"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="34" t="s">
+      <c r="F17" s="35"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="14"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A18" s="11"/>
+      <c r="B18" s="35"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="10"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A19" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="34" t="s">
+      <c r="B19" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="34" t="s">
+      <c r="C19" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="D19" s="34" t="s">
+      <c r="D19" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="E19" s="34" t="s">
+      <c r="E19" s="33" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="68" x14ac:dyDescent="0.2">
-      <c r="A20" s="34" t="s">
+      <c r="F19" s="10"/>
+    </row>
+    <row r="20" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+      <c r="A20" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="35" t="s">
+      <c r="B20" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="34" t="s">
+      <c r="C20" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="D20" s="34" t="s">
+      <c r="D20" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="E20" s="35" t="s">
+      <c r="E20" s="34" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A21" s="34" t="s">
+      <c r="F20" s="10"/>
+    </row>
+    <row r="21" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="A21" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="B21" s="35" t="s">
+      <c r="B21" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="C21" s="34"/>
-      <c r="D21" s="34" t="s">
+      <c r="C21" s="33"/>
+      <c r="D21" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="E21" s="35" t="s">
+      <c r="E21" s="34" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A22" s="34" t="s">
+      <c r="F21" s="10"/>
+    </row>
+    <row r="22" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="A22" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="34" t="s">
+      <c r="B22" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="34"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="35" t="s">
+      <c r="C22" s="33"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="34" t="s">
         <v>45</v>
       </c>
+      <c r="F22" s="10"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A23" s="11"/>
+      <c r="B23" s="35"/>
+      <c r="C23" s="35"/>
+      <c r="D23" s="35"/>
+      <c r="E23" s="35"/>
+      <c r="F23" s="10"/>
+    </row>
+    <row r="24" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="12"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Finished PCL extrusion temp testing and manual starve feeding
</commit_message>
<xml_diff>
--- a/Thesis Charts and Graphs.xlsx
+++ b/Thesis Charts and Graphs.xlsx
@@ -8,14 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://buckeyemailosu.sharepoint.com/sites/Tumortrackingresearch/Shared Documents/General/Theses/Isaac/Master's Thesis/ohio-state-coe-dissertation-template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="79" documentId="14_{BDDE5BD9-9B9B-1147-BD62-444B36ECC1DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E397CCAE-AE1B-464C-8EA5-F80EF5A09893}"/>
+  <xr:revisionPtr revIDLastSave="127" documentId="14_{BDDE5BD9-9B9B-1147-BD62-444B36ECC1DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{75F981D8-EA28-5D43-801E-8724871D8713}"/>
   <bookViews>
-    <workbookView xWindow="980" yWindow="500" windowWidth="34860" windowHeight="21900" activeTab="1" xr2:uid="{16E6A821-3DC4-194B-96AE-E7BDD0CEA9F6}"/>
+    <workbookView xWindow="980" yWindow="500" windowWidth="34860" windowHeight="21900" activeTab="2" xr2:uid="{16E6A821-3DC4-194B-96AE-E7BDD0CEA9F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="2" r:id="rId1"/>
     <sheet name="Literature Review" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$9:$A$21</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$B$8</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$B$8</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$B$9:$B$21</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$B$9:$B$21</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$A$9:$A$21</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$B$8</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$B$9:$B$21</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$A$9:$A$21</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$B$8</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$B$9:$B$21</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$A$9:$A$21</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="83">
   <si>
     <t>Seroma Visibility (RefID 25)</t>
   </si>
@@ -274,6 +289,30 @@
   </si>
   <si>
     <t>Standard Test Method for Tensile Properties of Plastics</t>
+  </si>
+  <si>
+    <t>Heater</t>
+  </si>
+  <si>
+    <t>Temperature (˚C)</t>
+  </si>
+  <si>
+    <t>H4</t>
+  </si>
+  <si>
+    <t>H3</t>
+  </si>
+  <si>
+    <t>H2</t>
+  </si>
+  <si>
+    <t>H1</t>
+  </si>
+  <si>
+    <t>Temperature</t>
+  </si>
+  <si>
+    <t>Extrudability</t>
   </si>
 </sst>
 </file>
@@ -576,7 +615,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -619,6 +658,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1152,7 +1192,413 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Extrudability</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$9:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>180</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$9:$B$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A967-7A48-9243-1F3FB88B61A9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="504348336"/>
+        <c:axId val="766442656"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="504348336"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="766442656"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="766442656"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="504348336"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1711,6 +2157,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1732,6 +2694,47 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4CFC9979-958C-7329-5F10-BC836EFE4FDA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>660400</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C9D9F43-CC4F-0346-67E1-B1A3E79EBBFD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2159,8 +3162,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDAF9E8A-4B25-1B41-82F3-06803E42F3DE}">
   <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F7" zoomScale="173" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView topLeftCell="E1" zoomScale="173" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19:J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2177,10 +3180,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32"/>
+      <c r="B1" s="33"/>
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
       <c r="E1" s="8"/>
@@ -2188,10 +3191,10 @@
       <c r="G1" s="8"/>
       <c r="H1" s="9"/>
       <c r="I1" s="8"/>
-      <c r="J1" s="37" t="s">
+      <c r="J1" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="K1" s="38" t="s">
+      <c r="K1" s="39" t="s">
         <v>61</v>
       </c>
       <c r="L1" s="9"/>
@@ -2203,13 +3206,13 @@
       <c r="B2" s="3">
         <v>8</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
       <c r="H2" s="10"/>
-      <c r="I2" s="35"/>
+      <c r="I2" s="36"/>
       <c r="J2" s="4" t="s">
         <v>50</v>
       </c>
@@ -2225,13 +3228,13 @@
       <c r="B3" s="5">
         <v>10</v>
       </c>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
       <c r="H3" s="10"/>
-      <c r="I3" s="35"/>
+      <c r="I3" s="36"/>
       <c r="J3" s="4" t="s">
         <v>52</v>
       </c>
@@ -2247,13 +3250,13 @@
       <c r="B4" s="5">
         <v>6</v>
       </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
       <c r="H4" s="10"/>
-      <c r="I4" s="35"/>
+      <c r="I4" s="36"/>
       <c r="J4" s="4" t="s">
         <v>54</v>
       </c>
@@ -2269,13 +3272,13 @@
       <c r="B5" s="7">
         <v>6</v>
       </c>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
       <c r="H5" s="10"/>
-      <c r="I5" s="35"/>
+      <c r="I5" s="36"/>
       <c r="J5" s="4" t="s">
         <v>56</v>
       </c>
@@ -2286,14 +3289,14 @@
     </row>
     <row r="6" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
+      <c r="B6" s="36"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
       <c r="H6" s="10"/>
-      <c r="I6" s="35"/>
+      <c r="I6" s="36"/>
       <c r="J6" s="6" t="s">
         <v>58</v>
       </c>
@@ -2304,40 +3307,40 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="11"/>
-      <c r="B7" s="35"/>
-      <c r="C7" s="35"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
+      <c r="B7" s="36"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
       <c r="H7" s="10"/>
-      <c r="I7" s="35"/>
-      <c r="J7" s="35"/>
-      <c r="K7" s="35"/>
+      <c r="I7" s="36"/>
+      <c r="J7" s="36"/>
+      <c r="K7" s="36"/>
       <c r="L7" s="10"/>
     </row>
     <row r="8" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11"/>
-      <c r="B8" s="35"/>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
+      <c r="B8" s="36"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
       <c r="H8" s="10"/>
-      <c r="I8" s="35"/>
-      <c r="J8" s="35"/>
-      <c r="K8" s="35"/>
+      <c r="I8" s="36"/>
+      <c r="J8" s="36"/>
+      <c r="K8" s="36"/>
       <c r="L8" s="10"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="11"/>
-      <c r="B9" s="35"/>
-      <c r="C9" s="35"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
+      <c r="B9" s="36"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
       <c r="H9" s="10"/>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
@@ -2346,16 +3349,16 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="11"/>
-      <c r="B10" s="35"/>
-      <c r="C10" s="35"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="35"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="36"/>
       <c r="H10" s="10"/>
-      <c r="I10" s="35"/>
-      <c r="J10" s="35"/>
-      <c r="K10" s="35"/>
+      <c r="I10" s="36"/>
+      <c r="J10" s="36"/>
+      <c r="K10" s="36"/>
       <c r="L10" s="10"/>
     </row>
     <row r="11" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -2367,11 +3370,11 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
       <c r="H11" s="14"/>
-      <c r="I11" s="35"/>
-      <c r="J11" s="35" t="s">
+      <c r="I11" s="36"/>
+      <c r="J11" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="K11" s="35" t="s">
+      <c r="K11" s="36" t="s">
         <v>63</v>
       </c>
       <c r="L11" s="10" t="s">
@@ -2380,18 +3383,18 @@
     </row>
     <row r="12" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11"/>
-      <c r="B12" s="35"/>
-      <c r="C12" s="35"/>
-      <c r="D12" s="35"/>
+      <c r="B12" s="36"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="36"/>
       <c r="E12" s="10"/>
-      <c r="F12" s="35"/>
+      <c r="F12" s="36"/>
       <c r="G12" s="11"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="35"/>
-      <c r="J12" s="35" t="s">
+      <c r="H12" s="36"/>
+      <c r="I12" s="36"/>
+      <c r="J12" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="K12" s="35" t="s">
+      <c r="K12" s="36" t="s">
         <v>65</v>
       </c>
       <c r="L12" s="10">
@@ -2399,27 +3402,27 @@
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="26" t="s">
+      <c r="A13" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="27" t="s">
+      <c r="C13" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="28" t="s">
+      <c r="D13" s="29" t="s">
         <v>22</v>
       </c>
       <c r="E13" s="10"/>
-      <c r="F13" s="35"/>
+      <c r="F13" s="36"/>
       <c r="G13" s="11"/>
-      <c r="H13" s="35"/>
-      <c r="I13" s="35"/>
-      <c r="J13" s="35" t="s">
+      <c r="H13" s="36"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="K13" s="35" t="s">
+      <c r="K13" s="36" t="s">
         <v>68</v>
       </c>
       <c r="L13" s="10">
@@ -2427,27 +3430,27 @@
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" s="29" t="s">
+      <c r="A14" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="24" t="s">
+      <c r="B14" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="24" t="s">
+      <c r="C14" s="25" t="s">
         <v>24</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>25</v>
       </c>
       <c r="E14" s="10"/>
-      <c r="F14" s="35"/>
+      <c r="F14" s="36"/>
       <c r="G14" s="11"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="35"/>
-      <c r="J14" s="35" t="s">
+      <c r="H14" s="36"/>
+      <c r="I14" s="36"/>
+      <c r="J14" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="K14" s="35" t="s">
+      <c r="K14" s="36" t="s">
         <v>70</v>
       </c>
       <c r="L14" s="10">
@@ -2455,27 +3458,27 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="29" t="s">
+      <c r="A15" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="24" t="s">
+      <c r="C15" s="25" t="s">
         <v>29</v>
       </c>
       <c r="D15" s="5">
         <v>-60</v>
       </c>
       <c r="E15" s="10"/>
-      <c r="F15" s="35"/>
+      <c r="F15" s="36"/>
       <c r="G15" s="11"/>
-      <c r="H15" s="35"/>
-      <c r="I15" s="35"/>
-      <c r="J15" s="35" t="s">
+      <c r="H15" s="36"/>
+      <c r="I15" s="36"/>
+      <c r="J15" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="K15" s="35" t="s">
+      <c r="K15" s="36" t="s">
         <v>72</v>
       </c>
       <c r="L15" s="10">
@@ -2483,27 +3486,27 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="30" t="s">
+      <c r="A16" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="25" t="s">
+      <c r="B16" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="25" t="s">
+      <c r="C16" s="26" t="s">
         <v>33</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>30</v>
       </c>
       <c r="E16" s="10"/>
-      <c r="F16" s="35"/>
+      <c r="F16" s="36"/>
       <c r="G16" s="11"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35" t="s">
+      <c r="H16" s="36"/>
+      <c r="I16" s="36"/>
+      <c r="J16" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="K16" s="35" t="s">
+      <c r="K16" s="36" t="s">
         <v>74</v>
       </c>
       <c r="L16" s="10">
@@ -2516,7 +3519,7 @@
       <c r="C17" s="13"/>
       <c r="D17" s="13"/>
       <c r="E17" s="14"/>
-      <c r="F17" s="35"/>
+      <c r="F17" s="36"/>
       <c r="G17" s="12"/>
       <c r="H17" s="13"/>
       <c r="I17" s="13"/>
@@ -2526,85 +3529,94 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="11"/>
-      <c r="B18" s="35"/>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35"/>
+      <c r="B18" s="36"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
       <c r="F18" s="10"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="9"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19" s="36" t="s">
+      <c r="A19" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="33" t="s">
+      <c r="B19" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="33" t="s">
+      <c r="C19" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="D19" s="33" t="s">
+      <c r="D19" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="E19" s="33" t="s">
+      <c r="E19" s="34" t="s">
         <v>37</v>
       </c>
       <c r="F19" s="10"/>
+      <c r="G19" s="11"/>
     </row>
     <row r="20" spans="1:12" ht="68" x14ac:dyDescent="0.2">
-      <c r="A20" s="36" t="s">
+      <c r="A20" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="34" t="s">
+      <c r="B20" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="33" t="s">
+      <c r="C20" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="D20" s="33" t="s">
+      <c r="D20" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="E20" s="34" t="s">
+      <c r="E20" s="35" t="s">
         <v>41</v>
       </c>
       <c r="F20" s="10"/>
+      <c r="G20" s="11"/>
     </row>
     <row r="21" spans="1:12" ht="34" x14ac:dyDescent="0.2">
-      <c r="A21" s="36" t="s">
+      <c r="A21" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="B21" s="34" t="s">
+      <c r="B21" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="C21" s="33"/>
-      <c r="D21" s="33" t="s">
+      <c r="C21" s="34"/>
+      <c r="D21" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="E21" s="34" t="s">
+      <c r="E21" s="35" t="s">
         <v>46</v>
       </c>
       <c r="F21" s="10"/>
+      <c r="G21" s="11"/>
     </row>
     <row r="22" spans="1:12" ht="34" x14ac:dyDescent="0.2">
-      <c r="A22" s="36" t="s">
+      <c r="A22" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="33" t="s">
+      <c r="B22" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="33"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="34" t="s">
+      <c r="C22" s="34"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="35" t="s">
         <v>45</v>
       </c>
       <c r="F22" s="10"/>
+      <c r="G22" s="11"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="11"/>
-      <c r="B23" s="35"/>
-      <c r="C23" s="35"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="35"/>
+      <c r="B23" s="36"/>
+      <c r="C23" s="36"/>
+      <c r="D23" s="36"/>
+      <c r="E23" s="36"/>
       <c r="F23" s="10"/>
+      <c r="G23" s="11"/>
     </row>
     <row r="24" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12"/>
@@ -2613,11 +3625,327 @@
       <c r="D24" s="13"/>
       <c r="E24" s="13"/>
       <c r="F24" s="14"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
   </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8738BA31-1A52-274A-92D6-B57235D8D2B5}">
+  <dimension ref="A1:I23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="9"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="36">
+        <v>140</v>
+      </c>
+      <c r="C2" s="10"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="36">
+        <v>155</v>
+      </c>
+      <c r="C3" s="10"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" s="36">
+        <v>160</v>
+      </c>
+      <c r="C4" s="10"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" s="36">
+        <v>160</v>
+      </c>
+      <c r="C5" s="10"/>
+    </row>
+    <row r="6" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="11"/>
+      <c r="B6" s="36"/>
+      <c r="C6" s="10"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="24"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="9"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" s="36" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="10"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="11">
+        <v>60</v>
+      </c>
+      <c r="B9" s="36">
+        <v>1</v>
+      </c>
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="36"/>
+      <c r="I9" s="10"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="11">
+        <v>70</v>
+      </c>
+      <c r="B10" s="36">
+        <v>1</v>
+      </c>
+      <c r="C10" s="36"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="10"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="11">
+        <v>80</v>
+      </c>
+      <c r="B11" s="36">
+        <v>2</v>
+      </c>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="10"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="11">
+        <v>90</v>
+      </c>
+      <c r="B12" s="36">
+        <v>2</v>
+      </c>
+      <c r="C12" s="36"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="10"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="11">
+        <v>100</v>
+      </c>
+      <c r="B13" s="36">
+        <v>2</v>
+      </c>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="10"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="11">
+        <v>110</v>
+      </c>
+      <c r="B14" s="36">
+        <v>2</v>
+      </c>
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="36"/>
+      <c r="I14" s="10"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="11">
+        <v>120</v>
+      </c>
+      <c r="B15" s="36">
+        <v>2</v>
+      </c>
+      <c r="C15" s="36"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="36"/>
+      <c r="I15" s="10"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="11">
+        <v>130</v>
+      </c>
+      <c r="B16" s="36">
+        <v>2</v>
+      </c>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="36"/>
+      <c r="I16" s="10"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="11">
+        <v>140</v>
+      </c>
+      <c r="B17" s="36">
+        <v>2</v>
+      </c>
+      <c r="C17" s="36"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="36"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="36"/>
+      <c r="I17" s="10"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="11">
+        <v>150</v>
+      </c>
+      <c r="B18" s="36">
+        <v>2</v>
+      </c>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="36"/>
+      <c r="I18" s="10"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="11">
+        <v>160</v>
+      </c>
+      <c r="B19" s="36">
+        <v>3</v>
+      </c>
+      <c r="C19" s="36"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="36"/>
+      <c r="G19" s="36"/>
+      <c r="H19" s="36"/>
+      <c r="I19" s="10"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="11">
+        <v>170</v>
+      </c>
+      <c r="B20" s="36">
+        <v>3</v>
+      </c>
+      <c r="C20" s="36"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="36"/>
+      <c r="G20" s="36"/>
+      <c r="H20" s="36"/>
+      <c r="I20" s="10"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="11">
+        <v>180</v>
+      </c>
+      <c r="B21" s="36">
+        <v>3</v>
+      </c>
+      <c r="C21" s="36"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="36"/>
+      <c r="H21" s="36"/>
+      <c r="I21" s="10"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="11"/>
+      <c r="B22" s="36"/>
+      <c r="C22" s="36"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="36"/>
+      <c r="F22" s="36"/>
+      <c r="G22" s="36"/>
+      <c r="H22" s="36"/>
+      <c r="I22" s="10"/>
+    </row>
+    <row r="23" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="12"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="14"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Working on starve feeding section of methodology
</commit_message>
<xml_diff>
--- a/Thesis Charts and Graphs.xlsx
+++ b/Thesis Charts and Graphs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://buckeyemailosu.sharepoint.com/sites/Tumortrackingresearch/Shared Documents/General/Theses/Isaac/Master's Thesis/ohio-state-coe-dissertation-template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="127" documentId="14_{BDDE5BD9-9B9B-1147-BD62-444B36ECC1DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{75F981D8-EA28-5D43-801E-8724871D8713}"/>
+  <xr:revisionPtr revIDLastSave="148" documentId="14_{BDDE5BD9-9B9B-1147-BD62-444B36ECC1DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C6F24E8F-7E7B-E145-88CE-73D0420F57FF}"/>
   <bookViews>
     <workbookView xWindow="980" yWindow="500" windowWidth="34860" windowHeight="21900" activeTab="2" xr2:uid="{16E6A821-3DC4-194B-96AE-E7BDD0CEA9F6}"/>
   </bookViews>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="95">
   <si>
     <t>Seroma Visibility (RefID 25)</t>
   </si>
@@ -313,6 +313,42 @@
   </si>
   <si>
     <t>Extrudability</t>
+  </si>
+  <si>
+    <t>Sourcing</t>
+  </si>
+  <si>
+    <t>Device Body</t>
+  </si>
+  <si>
+    <t>Ball Bearings</t>
+  </si>
+  <si>
+    <t>3D Printed (PLA)</t>
+  </si>
+  <si>
+    <t>Labs or 3D Printed (PLA)</t>
+  </si>
+  <si>
+    <t>Ring Stand</t>
+  </si>
+  <si>
+    <t>Labs</t>
+  </si>
+  <si>
+    <t>Stepper Motor</t>
+  </si>
+  <si>
+    <t>Gearbox</t>
+  </si>
+  <si>
+    <t>Drive Belt</t>
+  </si>
+  <si>
+    <t>3D Printed (TPU)</t>
+  </si>
+  <si>
+    <t>UI Components</t>
   </si>
 </sst>
 </file>
@@ -3641,15 +3677,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8738BA31-1A52-274A-92D6-B57235D8D2B5}">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="238" workbookViewId="0">
+      <selection activeCell="A32" sqref="A25:B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -3944,6 +3982,88 @@
       <c r="G23" s="13"/>
       <c r="H23" s="13"/>
       <c r="I23" s="14"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="24"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="9"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="C25" s="10"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="B26" s="36" t="s">
+        <v>86</v>
+      </c>
+      <c r="C26" s="10"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="B27" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="C27" s="10"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="B28" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="C28" s="10"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="B29" s="36" t="s">
+        <v>93</v>
+      </c>
+      <c r="C29" s="10"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="B30" s="36" t="s">
+        <v>89</v>
+      </c>
+      <c r="C30" s="10"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="B31" s="36" t="s">
+        <v>89</v>
+      </c>
+      <c r="C31" s="10"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="B32" s="36" t="s">
+        <v>89</v>
+      </c>
+      <c r="C32" s="10"/>
+    </row>
+    <row r="33" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="12"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Finished purging compounds section
</commit_message>
<xml_diff>
--- a/Thesis Charts and Graphs.xlsx
+++ b/Thesis Charts and Graphs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://buckeyemailosu.sharepoint.com/sites/Tumortrackingresearch/Shared Documents/General/Theses/Isaac/Master's Thesis/ohio-state-coe-dissertation-template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="148" documentId="14_{BDDE5BD9-9B9B-1147-BD62-444B36ECC1DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C6F24E8F-7E7B-E145-88CE-73D0420F57FF}"/>
+  <xr:revisionPtr revIDLastSave="158" documentId="14_{BDDE5BD9-9B9B-1147-BD62-444B36ECC1DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{25423FF1-6194-7F4F-9DDF-DBD1CEF6BAE5}"/>
   <bookViews>
     <workbookView xWindow="980" yWindow="500" windowWidth="34860" windowHeight="21900" activeTab="2" xr2:uid="{16E6A821-3DC4-194B-96AE-E7BDD0CEA9F6}"/>
   </bookViews>
@@ -17,20 +17,6 @@
     <sheet name="Literature Review" sheetId="1" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$9:$A$21</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$B$8</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$B$8</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$B$9:$B$21</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$B$9:$B$21</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$A$9:$A$21</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$B$8</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$B$9:$B$21</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$A$9:$A$21</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$B$8</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$B$9:$B$21</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$A$9:$A$21</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -52,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="102">
   <si>
     <t>Seroma Visibility (RefID 25)</t>
   </si>
@@ -349,6 +335,27 @@
   </si>
   <si>
     <t>UI Components</t>
+  </si>
+  <si>
+    <t>Purging Compound</t>
+  </si>
+  <si>
+    <t>Ideal Material</t>
+  </si>
+  <si>
+    <t>Requires HDPE</t>
+  </si>
+  <si>
+    <t>DP-D2</t>
+  </si>
+  <si>
+    <t>DP-L</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -702,19 +709,12 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -724,6 +724,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3216,10 +3223,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33"/>
+      <c r="B1" s="38"/>
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
       <c r="E1" s="8"/>
@@ -3227,10 +3234,10 @@
       <c r="G1" s="8"/>
       <c r="H1" s="9"/>
       <c r="I1" s="8"/>
-      <c r="J1" s="38" t="s">
+      <c r="J1" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="K1" s="39" t="s">
+      <c r="K1" s="36" t="s">
         <v>61</v>
       </c>
       <c r="L1" s="9"/>
@@ -3242,13 +3249,7 @@
       <c r="B2" s="3">
         <v>8</v>
       </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
       <c r="H2" s="10"/>
-      <c r="I2" s="36"/>
       <c r="J2" s="4" t="s">
         <v>50</v>
       </c>
@@ -3264,13 +3265,7 @@
       <c r="B3" s="5">
         <v>10</v>
       </c>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
       <c r="H3" s="10"/>
-      <c r="I3" s="36"/>
       <c r="J3" s="4" t="s">
         <v>52</v>
       </c>
@@ -3286,13 +3281,7 @@
       <c r="B4" s="5">
         <v>6</v>
       </c>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
       <c r="H4" s="10"/>
-      <c r="I4" s="36"/>
       <c r="J4" s="4" t="s">
         <v>54</v>
       </c>
@@ -3308,13 +3297,7 @@
       <c r="B5" s="7">
         <v>6</v>
       </c>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
       <c r="H5" s="10"/>
-      <c r="I5" s="36"/>
       <c r="J5" s="4" t="s">
         <v>56</v>
       </c>
@@ -3325,14 +3308,7 @@
     </row>
     <row r="6" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
-      <c r="B6" s="36"/>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
-      <c r="G6" s="36"/>
       <c r="H6" s="10"/>
-      <c r="I6" s="36"/>
       <c r="J6" s="6" t="s">
         <v>58</v>
       </c>
@@ -3343,40 +3319,16 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="11"/>
-      <c r="B7" s="36"/>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
-      <c r="G7" s="36"/>
       <c r="H7" s="10"/>
-      <c r="I7" s="36"/>
-      <c r="J7" s="36"/>
-      <c r="K7" s="36"/>
       <c r="L7" s="10"/>
     </row>
     <row r="8" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11"/>
-      <c r="B8" s="36"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
       <c r="H8" s="10"/>
-      <c r="I8" s="36"/>
-      <c r="J8" s="36"/>
-      <c r="K8" s="36"/>
       <c r="L8" s="10"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="11"/>
-      <c r="B9" s="36"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
       <c r="H9" s="10"/>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
@@ -3385,16 +3337,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="11"/>
-      <c r="B10" s="36"/>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36"/>
       <c r="H10" s="10"/>
-      <c r="I10" s="36"/>
-      <c r="J10" s="36"/>
-      <c r="K10" s="36"/>
       <c r="L10" s="10"/>
     </row>
     <row r="11" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -3406,11 +3349,10 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
       <c r="H11" s="14"/>
-      <c r="I11" s="36"/>
-      <c r="J11" s="36" t="s">
+      <c r="J11" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="K11" s="36" t="s">
+      <c r="K11" s="1" t="s">
         <v>63</v>
       </c>
       <c r="L11" s="10" t="s">
@@ -3419,18 +3361,12 @@
     </row>
     <row r="12" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11"/>
-      <c r="B12" s="36"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
       <c r="E12" s="10"/>
-      <c r="F12" s="36"/>
       <c r="G12" s="11"/>
-      <c r="H12" s="36"/>
-      <c r="I12" s="36"/>
-      <c r="J12" s="36" t="s">
+      <c r="J12" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="K12" s="36" t="s">
+      <c r="K12" s="1" t="s">
         <v>65</v>
       </c>
       <c r="L12" s="10">
@@ -3451,14 +3387,11 @@
         <v>22</v>
       </c>
       <c r="E13" s="10"/>
-      <c r="F13" s="36"/>
       <c r="G13" s="11"/>
-      <c r="H13" s="36"/>
-      <c r="I13" s="36"/>
-      <c r="J13" s="36" t="s">
+      <c r="J13" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="K13" s="36" t="s">
+      <c r="K13" s="1" t="s">
         <v>68</v>
       </c>
       <c r="L13" s="10">
@@ -3479,14 +3412,11 @@
         <v>25</v>
       </c>
       <c r="E14" s="10"/>
-      <c r="F14" s="36"/>
       <c r="G14" s="11"/>
-      <c r="H14" s="36"/>
-      <c r="I14" s="36"/>
-      <c r="J14" s="36" t="s">
+      <c r="J14" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="K14" s="36" t="s">
+      <c r="K14" s="1" t="s">
         <v>70</v>
       </c>
       <c r="L14" s="10">
@@ -3507,14 +3437,11 @@
         <v>-60</v>
       </c>
       <c r="E15" s="10"/>
-      <c r="F15" s="36"/>
       <c r="G15" s="11"/>
-      <c r="H15" s="36"/>
-      <c r="I15" s="36"/>
-      <c r="J15" s="36" t="s">
+      <c r="J15" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="K15" s="36" t="s">
+      <c r="K15" s="1" t="s">
         <v>72</v>
       </c>
       <c r="L15" s="10">
@@ -3535,14 +3462,11 @@
         <v>30</v>
       </c>
       <c r="E16" s="10"/>
-      <c r="F16" s="36"/>
       <c r="G16" s="11"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="36"/>
-      <c r="J16" s="36" t="s">
+      <c r="J16" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="K16" s="36" t="s">
+      <c r="K16" s="1" t="s">
         <v>74</v>
       </c>
       <c r="L16" s="10">
@@ -3555,7 +3479,6 @@
       <c r="C17" s="13"/>
       <c r="D17" s="13"/>
       <c r="E17" s="14"/>
-      <c r="F17" s="36"/>
       <c r="G17" s="12"/>
       <c r="H17" s="13"/>
       <c r="I17" s="13"/>
@@ -3565,10 +3488,6 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="11"/>
-      <c r="B18" s="36"/>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
       <c r="F18" s="10"/>
       <c r="G18" s="24"/>
       <c r="H18" s="8"/>
@@ -3576,70 +3495,70 @@
       <c r="J18" s="9"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19" s="37" t="s">
+      <c r="A19" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="34" t="s">
+      <c r="B19" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="34" t="s">
+      <c r="C19" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="D19" s="34" t="s">
+      <c r="D19" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="E19" s="34" t="s">
+      <c r="E19" s="32" t="s">
         <v>37</v>
       </c>
       <c r="F19" s="10"/>
       <c r="G19" s="11"/>
     </row>
     <row r="20" spans="1:12" ht="68" x14ac:dyDescent="0.2">
-      <c r="A20" s="37" t="s">
+      <c r="A20" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="35" t="s">
+      <c r="B20" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="34" t="s">
+      <c r="C20" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="D20" s="34" t="s">
+      <c r="D20" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="E20" s="35" t="s">
+      <c r="E20" s="33" t="s">
         <v>41</v>
       </c>
       <c r="F20" s="10"/>
       <c r="G20" s="11"/>
     </row>
     <row r="21" spans="1:12" ht="34" x14ac:dyDescent="0.2">
-      <c r="A21" s="37" t="s">
+      <c r="A21" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="B21" s="35" t="s">
+      <c r="B21" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="C21" s="34"/>
-      <c r="D21" s="34" t="s">
+      <c r="C21" s="32"/>
+      <c r="D21" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="E21" s="35" t="s">
+      <c r="E21" s="33" t="s">
         <v>46</v>
       </c>
       <c r="F21" s="10"/>
       <c r="G21" s="11"/>
     </row>
     <row r="22" spans="1:12" ht="34" x14ac:dyDescent="0.2">
-      <c r="A22" s="37" t="s">
+      <c r="A22" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="34" t="s">
+      <c r="B22" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="34"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="35" t="s">
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="33" t="s">
         <v>45</v>
       </c>
       <c r="F22" s="10"/>
@@ -3647,10 +3566,6 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="11"/>
-      <c r="B23" s="36"/>
-      <c r="C23" s="36"/>
-      <c r="D23" s="36"/>
-      <c r="E23" s="36"/>
       <c r="F23" s="10"/>
       <c r="G23" s="11"/>
     </row>
@@ -3680,7 +3595,7 @@
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScale="238" workbookViewId="0">
-      <selection activeCell="A32" sqref="A25:B32"/>
+      <selection activeCell="D25" sqref="D25:F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3703,7 +3618,7 @@
       <c r="A2" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="36">
+      <c r="B2" s="1">
         <v>140</v>
       </c>
       <c r="C2" s="10"/>
@@ -3712,7 +3627,7 @@
       <c r="A3" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="B3" s="36">
+      <c r="B3" s="1">
         <v>155</v>
       </c>
       <c r="C3" s="10"/>
@@ -3721,7 +3636,7 @@
       <c r="A4" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="B4" s="36">
+      <c r="B4" s="1">
         <v>160</v>
       </c>
       <c r="C4" s="10"/>
@@ -3730,14 +3645,13 @@
       <c r="A5" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="B5" s="36">
+      <c r="B5" s="1">
         <v>160</v>
       </c>
       <c r="C5" s="10"/>
     </row>
     <row r="6" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
-      <c r="B6" s="36"/>
       <c r="C6" s="10"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -3755,221 +3669,130 @@
       <c r="A8" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="36"/>
       <c r="I8" s="10"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="11">
         <v>60</v>
       </c>
-      <c r="B9" s="36">
+      <c r="B9" s="1">
         <v>1</v>
       </c>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="36"/>
       <c r="I9" s="10"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="11">
         <v>70</v>
       </c>
-      <c r="B10" s="36">
+      <c r="B10" s="1">
         <v>1</v>
       </c>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
       <c r="I10" s="10"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="11">
         <v>80</v>
       </c>
-      <c r="B11" s="36">
+      <c r="B11" s="1">
         <v>2</v>
       </c>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="36"/>
-      <c r="H11" s="36"/>
       <c r="I11" s="10"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
         <v>90</v>
       </c>
-      <c r="B12" s="36">
+      <c r="B12" s="1">
         <v>2</v>
       </c>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="36"/>
       <c r="I12" s="10"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="11">
         <v>100</v>
       </c>
-      <c r="B13" s="36">
+      <c r="B13" s="1">
         <v>2</v>
       </c>
-      <c r="C13" s="36"/>
-      <c r="D13" s="36"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="36"/>
-      <c r="G13" s="36"/>
-      <c r="H13" s="36"/>
       <c r="I13" s="10"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="11">
         <v>110</v>
       </c>
-      <c r="B14" s="36">
+      <c r="B14" s="1">
         <v>2</v>
       </c>
-      <c r="C14" s="36"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="36"/>
       <c r="I14" s="10"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="11">
         <v>120</v>
       </c>
-      <c r="B15" s="36">
+      <c r="B15" s="1">
         <v>2</v>
       </c>
-      <c r="C15" s="36"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="36"/>
       <c r="I15" s="10"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="11">
         <v>130</v>
       </c>
-      <c r="B16" s="36">
+      <c r="B16" s="1">
         <v>2</v>
       </c>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="36"/>
       <c r="I16" s="10"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="11">
         <v>140</v>
       </c>
-      <c r="B17" s="36">
+      <c r="B17" s="1">
         <v>2</v>
       </c>
-      <c r="C17" s="36"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="36"/>
       <c r="I17" s="10"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="11">
         <v>150</v>
       </c>
-      <c r="B18" s="36">
+      <c r="B18" s="1">
         <v>2</v>
       </c>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="36"/>
       <c r="I18" s="10"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="11">
         <v>160</v>
       </c>
-      <c r="B19" s="36">
+      <c r="B19" s="1">
         <v>3</v>
       </c>
-      <c r="C19" s="36"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="36"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="36"/>
-      <c r="H19" s="36"/>
       <c r="I19" s="10"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="11">
         <v>170</v>
       </c>
-      <c r="B20" s="36">
+      <c r="B20" s="1">
         <v>3</v>
       </c>
-      <c r="C20" s="36"/>
-      <c r="D20" s="36"/>
-      <c r="E20" s="36"/>
-      <c r="F20" s="36"/>
-      <c r="G20" s="36"/>
-      <c r="H20" s="36"/>
       <c r="I20" s="10"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="11">
         <v>180</v>
       </c>
-      <c r="B21" s="36">
+      <c r="B21" s="1">
         <v>3</v>
       </c>
-      <c r="C21" s="36"/>
-      <c r="D21" s="36"/>
-      <c r="E21" s="36"/>
-      <c r="F21" s="36"/>
-      <c r="G21" s="36"/>
-      <c r="H21" s="36"/>
       <c r="I21" s="10"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="11"/>
-      <c r="B22" s="36"/>
-      <c r="C22" s="36"/>
-      <c r="D22" s="36"/>
-      <c r="E22" s="36"/>
-      <c r="F22" s="36"/>
-      <c r="G22" s="36"/>
-      <c r="H22" s="36"/>
       <c r="I22" s="10"/>
     </row>
     <row r="23" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -3987,48 +3810,86 @@
       <c r="A24" s="24"/>
       <c r="B24" s="8"/>
       <c r="C24" s="9"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="9"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="36" t="s">
+      <c r="B25" s="1" t="s">
         <v>83</v>
       </c>
       <c r="C25" s="10"/>
+      <c r="D25" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E25" s="39" t="s">
+        <v>96</v>
+      </c>
+      <c r="F25" s="39" t="s">
+        <v>97</v>
+      </c>
+      <c r="G25" s="10"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="B26" s="36" t="s">
+      <c r="B26" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C26" s="10"/>
+      <c r="D26" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="E26" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="F26" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="G26" s="10"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="B27" s="36" t="s">
+      <c r="B27" s="1" t="s">
         <v>87</v>
       </c>
       <c r="C27" s="10"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D27" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="E27" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="F27" s="39" t="s">
+        <v>101</v>
+      </c>
+      <c r="G27" s="10"/>
+    </row>
+    <row r="28" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="B28" s="36" t="s">
+      <c r="B28" s="1" t="s">
         <v>87</v>
       </c>
       <c r="C28" s="10"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="14"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="B29" s="36" t="s">
+      <c r="B29" s="1" t="s">
         <v>93</v>
       </c>
       <c r="C29" s="10"/>
@@ -4037,7 +3898,7 @@
       <c r="A30" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="B30" s="36" t="s">
+      <c r="B30" s="1" t="s">
         <v>89</v>
       </c>
       <c r="C30" s="10"/>
@@ -4046,7 +3907,7 @@
       <c r="A31" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="B31" s="36" t="s">
+      <c r="B31" s="1" t="s">
         <v>89</v>
       </c>
       <c r="C31" s="10"/>
@@ -4055,7 +3916,7 @@
       <c r="A32" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="B32" s="36" t="s">
+      <c r="B32" s="1" t="s">
         <v>89</v>
       </c>
       <c r="C32" s="10"/>
@@ -4067,6 +3928,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -4081,17 +3943,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="40c2d214-4ca5-4604-be72-e6c4439e5276">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="581c75f3-c23e-4d61-ac2d-458e1df0a137" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010020A0C45D55D81B409E1ED58F2E9DADA4" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4fa2050de8fd1970c7139c0348e41ca3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="40c2d214-4ca5-4604-be72-e6c4439e5276" xmlns:ns3="581c75f3-c23e-4d61-ac2d-458e1df0a137" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f9a6f9f6c893a0ba7e28c007d9267f0e" ns2:_="" ns3:_="">
     <xsd:import namespace="40c2d214-4ca5-4604-be72-e6c4439e5276"/>
@@ -4298,6 +4149,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="40c2d214-4ca5-4604-be72-e6c4439e5276">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="581c75f3-c23e-4d61-ac2d-458e1df0a137" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77CBFA7D-3A0A-48A4-8B12-895234E5D6E5}">
   <ds:schemaRefs>
@@ -4307,23 +4169,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F17E70AE-5CD9-46AD-9CD7-253B7D5337F5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="581c75f3-c23e-4d61-ac2d-458e1df0a137"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="40c2d214-4ca5-4604-be72-e6c4439e5276"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDAD4442-CD32-4282-A934-0FFE683B5B87}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4340,4 +4185,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F17E70AE-5CD9-46AD-9CD7-253B7D5337F5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="581c75f3-c23e-4d61-ac2d-458e1df0a137"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="40c2d214-4ca5-4604-be72-e6c4439e5276"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Finished BaSO4 extrusion sections
</commit_message>
<xml_diff>
--- a/Thesis Charts and Graphs.xlsx
+++ b/Thesis Charts and Graphs.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://buckeyemailosu.sharepoint.com/sites/Tumortrackingresearch/Shared Documents/General/Theses/Isaac/Master's Thesis/ohio-state-coe-dissertation-template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="158" documentId="14_{BDDE5BD9-9B9B-1147-BD62-444B36ECC1DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{25423FF1-6194-7F4F-9DDF-DBD1CEF6BAE5}"/>
+  <xr:revisionPtr revIDLastSave="186" documentId="14_{BDDE5BD9-9B9B-1147-BD62-444B36ECC1DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EA2196E9-9ACC-444D-9515-E1BCF12F016D}"/>
   <bookViews>
     <workbookView xWindow="980" yWindow="500" windowWidth="34860" windowHeight="21900" activeTab="2" xr2:uid="{16E6A821-3DC4-194B-96AE-E7BDD0CEA9F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="2" r:id="rId1"/>
     <sheet name="Literature Review" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
+    <sheet name="Methodology" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="106">
   <si>
     <t>Seroma Visibility (RefID 25)</t>
   </si>
@@ -356,6 +356,18 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>Percentage of BaSO4</t>
+  </si>
+  <si>
+    <t>Average Filament Thickness (mm)</t>
+  </si>
+  <si>
+    <t>Starting Time (s)</t>
+  </si>
+  <si>
+    <t>Ending Time (s)</t>
   </si>
 </sst>
 </file>
@@ -1290,7 +1302,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$8</c:f>
+              <c:f>Methodology!$B$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1313,7 +1325,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$9:$A$21</c:f>
+              <c:f>Methodology!$A$9:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1361,7 +1373,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$9:$B$21</c:f>
+              <c:f>Methodology!$B$9:$B$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -3592,10 +3604,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8738BA31-1A52-274A-92D6-B57235D8D2B5}">
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScale="238" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25:F27"/>
+      <selection activeCell="E35" sqref="D30:G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3902,6 +3914,18 @@
         <v>89</v>
       </c>
       <c r="C30" s="10"/>
+      <c r="D30" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
@@ -3911,6 +3935,18 @@
         <v>89</v>
       </c>
       <c r="C31" s="10"/>
+      <c r="D31" s="1">
+        <v>0</v>
+      </c>
+      <c r="E31" s="1">
+        <v>1.754</v>
+      </c>
+      <c r="F31" s="1">
+        <v>200</v>
+      </c>
+      <c r="G31" s="1">
+        <v>2500</v>
+      </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
@@ -3920,11 +3956,63 @@
         <v>89</v>
       </c>
       <c r="C32" s="10"/>
-    </row>
-    <row r="33" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D32" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="E32" s="1">
+        <v>1.778</v>
+      </c>
+      <c r="F32" s="1">
+        <v>1250</v>
+      </c>
+      <c r="G32" s="1">
+        <v>1960</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="12"/>
       <c r="B33" s="13"/>
       <c r="C33" s="14"/>
+      <c r="D33" s="1">
+        <v>5</v>
+      </c>
+      <c r="E33" s="1">
+        <v>1.738</v>
+      </c>
+      <c r="F33" s="1">
+        <v>1000</v>
+      </c>
+      <c r="G33" s="1">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D34" s="1">
+        <v>7.5</v>
+      </c>
+      <c r="E34" s="1">
+        <v>1.75</v>
+      </c>
+      <c r="F34" s="1">
+        <v>750</v>
+      </c>
+      <c r="G34" s="1">
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D35" s="1">
+        <v>10</v>
+      </c>
+      <c r="E35" s="1">
+        <v>1.754</v>
+      </c>
+      <c r="F35" s="1">
+        <v>450</v>
+      </c>
+      <c r="G35" s="1">
+        <v>1300</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Finished 3D printing PLCL
</commit_message>
<xml_diff>
--- a/Thesis Charts and Graphs.xlsx
+++ b/Thesis Charts and Graphs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://buckeyemailosu.sharepoint.com/sites/Tumortrackingresearch/Shared Documents/General/Theses/Isaac/Master's Thesis/ohio-state-coe-dissertation-template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="186" documentId="14_{BDDE5BD9-9B9B-1147-BD62-444B36ECC1DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EA2196E9-9ACC-444D-9515-E1BCF12F016D}"/>
+  <xr:revisionPtr revIDLastSave="189" documentId="14_{BDDE5BD9-9B9B-1147-BD62-444B36ECC1DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1B0280F8-BCD2-9742-9B8F-59F8D7A5AACE}"/>
   <bookViews>
     <workbookView xWindow="980" yWindow="500" windowWidth="34860" windowHeight="21900" activeTab="2" xr2:uid="{16E6A821-3DC4-194B-96AE-E7BDD0CEA9F6}"/>
   </bookViews>
@@ -3604,10 +3604,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8738BA31-1A52-274A-92D6-B57235D8D2B5}">
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="238" workbookViewId="0">
-      <selection activeCell="E35" sqref="D30:G35"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="238" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3892,10 +3892,10 @@
         <v>87</v>
       </c>
       <c r="C28" s="10"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="14"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="39"/>
+      <c r="F28" s="39"/>
+      <c r="G28" s="10"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
@@ -3904,7 +3904,12 @@
       <c r="B29" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C29" s="10"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="24"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="9"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
@@ -3913,19 +3918,20 @@
       <c r="B30" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C30" s="10"/>
-      <c r="D30" s="1" t="s">
+      <c r="C30" s="39"/>
+      <c r="D30" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="E30" s="39" t="s">
         <v>103</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="F30" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="G30" s="1" t="s">
+      <c r="G30" s="39" t="s">
         <v>105</v>
       </c>
+      <c r="H30" s="10"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
@@ -3934,19 +3940,20 @@
       <c r="B31" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C31" s="10"/>
-      <c r="D31" s="1">
+      <c r="C31" s="39"/>
+      <c r="D31" s="11">
         <v>0</v>
       </c>
-      <c r="E31" s="1">
+      <c r="E31" s="39">
         <v>1.754</v>
       </c>
-      <c r="F31" s="1">
+      <c r="F31" s="39">
         <v>200</v>
       </c>
-      <c r="G31" s="1">
+      <c r="G31" s="39">
         <v>2500</v>
       </c>
+      <c r="H31" s="10"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
@@ -3955,64 +3962,75 @@
       <c r="B32" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C32" s="10"/>
-      <c r="D32" s="1">
+      <c r="C32" s="39"/>
+      <c r="D32" s="11">
         <v>2.5</v>
       </c>
-      <c r="E32" s="1">
+      <c r="E32" s="39">
         <v>1.778</v>
       </c>
-      <c r="F32" s="1">
+      <c r="F32" s="39">
         <v>1250</v>
       </c>
-      <c r="G32" s="1">
+      <c r="G32" s="39">
         <v>1960</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="H32" s="10"/>
+    </row>
+    <row r="33" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="12"/>
       <c r="B33" s="13"/>
-      <c r="C33" s="14"/>
-      <c r="D33" s="1">
+      <c r="C33" s="13"/>
+      <c r="D33" s="11">
         <v>5</v>
       </c>
-      <c r="E33" s="1">
+      <c r="E33" s="39">
         <v>1.738</v>
       </c>
-      <c r="F33" s="1">
+      <c r="F33" s="39">
         <v>1000</v>
       </c>
-      <c r="G33" s="1">
+      <c r="G33" s="39">
         <v>2400</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D34" s="1">
+      <c r="H33" s="10"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D34" s="11">
         <v>7.5</v>
       </c>
-      <c r="E34" s="1">
+      <c r="E34" s="39">
         <v>1.75</v>
       </c>
-      <c r="F34" s="1">
+      <c r="F34" s="39">
         <v>750</v>
       </c>
-      <c r="G34" s="1">
+      <c r="G34" s="39">
         <v>1900</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D35" s="1">
+      <c r="H34" s="10"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D35" s="11">
         <v>10</v>
       </c>
-      <c r="E35" s="1">
+      <c r="E35" s="39">
         <v>1.754</v>
       </c>
-      <c r="F35" s="1">
+      <c r="F35" s="39">
         <v>450</v>
       </c>
-      <c r="G35" s="1">
+      <c r="G35" s="39">
         <v>1300</v>
       </c>
+      <c r="H35" s="10"/>
+    </row>
+    <row r="36" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D36" s="12"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4031,8 +4049,8 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010020A0C45D55D81B409E1ED58F2E9DADA4" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4fa2050de8fd1970c7139c0348e41ca3">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="40c2d214-4ca5-4604-be72-e6c4439e5276" xmlns:ns3="581c75f3-c23e-4d61-ac2d-458e1df0a137" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f9a6f9f6c893a0ba7e28c007d9267f0e" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010020A0C45D55D81B409E1ED58F2E9DADA4" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b3439157d04fb2c0c2146dbea8d1ca4f">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="40c2d214-4ca5-4604-be72-e6c4439e5276" xmlns:ns3="581c75f3-c23e-4d61-ac2d-458e1df0a137" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4c3248ab5c1b5bd60be37440245572d8" ns2:_="" ns3:_="">
     <xsd:import namespace="40c2d214-4ca5-4604-be72-e6c4439e5276"/>
     <xsd:import namespace="581c75f3-c23e-4d61-ac2d-458e1df0a137"/>
     <xsd:element name="properties">
@@ -4257,22 +4275,7 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDAD4442-CD32-4282-A934-0FFE683B5B87}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="40c2d214-4ca5-4604-be72-e6c4439e5276"/>
-    <ds:schemaRef ds:uri="581c75f3-c23e-4d61-ac2d-458e1df0a137"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{548D2A98-E4BA-493B-BDDF-E4239C4502BF}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
Working on external labs section, fixed appendix formatting
</commit_message>
<xml_diff>
--- a/Thesis Charts and Graphs.xlsx
+++ b/Thesis Charts and Graphs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://buckeyemailosu.sharepoint.com/sites/Tumortrackingresearch/Shared Documents/General/Theses/Isaac/Master's Thesis/ohio-state-coe-dissertation-template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="189" documentId="14_{BDDE5BD9-9B9B-1147-BD62-444B36ECC1DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1B0280F8-BCD2-9742-9B8F-59F8D7A5AACE}"/>
+  <xr:revisionPtr revIDLastSave="220" documentId="14_{BDDE5BD9-9B9B-1147-BD62-444B36ECC1DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6ADE7D6F-6544-AE49-9E4F-9DD574D2020B}"/>
   <bookViews>
     <workbookView xWindow="980" yWindow="500" windowWidth="34860" windowHeight="21900" activeTab="2" xr2:uid="{16E6A821-3DC4-194B-96AE-E7BDD0CEA9F6}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="126">
   <si>
     <t>Seroma Visibility (RefID 25)</t>
   </si>
@@ -368,6 +368,75 @@
   </si>
   <si>
     <t>Ending Time (s)</t>
+  </si>
+  <si>
+    <t>Lab</t>
+  </si>
+  <si>
+    <t>Research Assistance</t>
+  </si>
+  <si>
+    <t>Relevant Sections in Thesis</t>
+  </si>
+  <si>
+    <t>Polymer Synthesis Research Facility (PSRF)</t>
+  </si>
+  <si>
+    <t>- GPC testing
+- Material drying pre-extrusion
+- Discussion on methods to chemically combine PLA and PCL
+- Able to borrow a mortar and pestle to explore pulverizing filament options</t>
+  </si>
+  <si>
+    <t>Stephanie Spielman Comprehensive Cancer Center (OSUCCC)</t>
+  </si>
+  <si>
+    <t>- Conducted all imaging studies and analysis</t>
+  </si>
+  <si>
+    <t>Center for Design and Manufacturing Excellence (CDME)</t>
+  </si>
+  <si>
+    <t>- Tensile and Flexural testing
+- Observed filament regrinding capabilities</t>
+  </si>
+  <si>
+    <t>College of Pharmacy</t>
+  </si>
+  <si>
+    <t>- Toured research facilities
+- Discussed methods of creating a homogenous mixture</t>
+  </si>
+  <si>
+    <t>Engineering Education Department (EED)</t>
+  </si>
+  <si>
+    <t>- 3D printer troubleshooting
+- Able to borrow a Bambu P1P for initial testing</t>
+  </si>
+  <si>
+    <t>Industrial and Systems Engineering Department (ISE)</t>
+  </si>
+  <si>
+    <t>- Discussed various extrusion questions and troubleshooting
+- Able to use supply of HDPE pellets for initial testing</t>
+  </si>
+  <si>
+    <t>Gear Lab</t>
+  </si>
+  <si>
+    <t>- Discussed various gear system questions
+- Helped brainstorm modifications to starve feeder system
+- Able to use existing gear and belt system for a more robust drive system</t>
+  </si>
+  <si>
+    <t>1, 2</t>
+  </si>
+  <si>
+    <t>3, 4</t>
+  </si>
+  <si>
+    <t>1, 7</t>
   </si>
 </sst>
 </file>
@@ -670,7 +739,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -742,7 +811,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3604,20 +3679,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8738BA31-1A52-274A-92D6-B57235D8D2B5}">
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="238" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" topLeftCell="J5" zoomScale="238" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.83203125" style="1"/>
+    <col min="3" max="10" width="10.83203125" style="1"/>
+    <col min="11" max="11" width="31" style="1" customWidth="1"/>
+    <col min="12" max="12" width="28.33203125" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
         <v>75</v>
       </c>
@@ -3625,8 +3703,17 @@
         <v>76</v>
       </c>
       <c r="C1" s="9"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="119" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>77</v>
       </c>
@@ -3634,8 +3721,17 @@
         <v>140</v>
       </c>
       <c r="C2" s="10"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K2" s="41" t="s">
+        <v>109</v>
+      </c>
+      <c r="L2" s="39" t="s">
+        <v>110</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>78</v>
       </c>
@@ -3643,8 +3739,17 @@
         <v>155</v>
       </c>
       <c r="C3" s="10"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K3" s="41" t="s">
+        <v>111</v>
+      </c>
+      <c r="L3" s="40" t="s">
+        <v>112</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>79</v>
       </c>
@@ -3652,8 +3757,14 @@
         <v>160</v>
       </c>
       <c r="C4" s="10"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K4" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="L4" s="39" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>80</v>
       </c>
@@ -3661,12 +3772,27 @@
         <v>160</v>
       </c>
       <c r="C5" s="10"/>
-    </row>
-    <row r="6" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K5" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="L5" s="39" t="s">
+        <v>116</v>
+      </c>
+      <c r="M5" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="52" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
       <c r="C6" s="10"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K6" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L6" s="39" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="68" x14ac:dyDescent="0.2">
       <c r="A7" s="24"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
@@ -3676,8 +3802,17 @@
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
       <c r="I7" s="9"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K7" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="L7" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="136" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
         <v>81</v>
       </c>
@@ -3685,8 +3820,14 @@
         <v>82</v>
       </c>
       <c r="I8" s="10"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K8" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="L8" s="39" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="11">
         <v>60</v>
       </c>
@@ -3695,7 +3836,7 @@
       </c>
       <c r="I9" s="10"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="11">
         <v>70</v>
       </c>
@@ -3704,7 +3845,7 @@
       </c>
       <c r="I10" s="10"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="11">
         <v>80</v>
       </c>
@@ -3713,7 +3854,7 @@
       </c>
       <c r="I11" s="10"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
         <v>90</v>
       </c>
@@ -3722,7 +3863,7 @@
       </c>
       <c r="I12" s="10"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="11">
         <v>100</v>
       </c>
@@ -3731,7 +3872,7 @@
       </c>
       <c r="I13" s="10"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="11">
         <v>110</v>
       </c>
@@ -3740,7 +3881,7 @@
       </c>
       <c r="I14" s="10"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="11">
         <v>120</v>
       </c>
@@ -3749,7 +3890,7 @@
       </c>
       <c r="I15" s="10"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="11">
         <v>130</v>
       </c>
@@ -3838,10 +3979,10 @@
       <c r="D25" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="E25" s="39" t="s">
+      <c r="E25" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="F25" s="39" t="s">
+      <c r="F25" s="1" t="s">
         <v>97</v>
       </c>
       <c r="G25" s="10"/>
@@ -3857,10 +3998,10 @@
       <c r="D26" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="E26" s="39" t="s">
+      <c r="E26" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F26" s="39" t="s">
+      <c r="F26" s="1" t="s">
         <v>100</v>
       </c>
       <c r="G26" s="10"/>
@@ -3876,10 +4017,10 @@
       <c r="D27" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="E27" s="39" t="s">
+      <c r="E27" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F27" s="39" t="s">
+      <c r="F27" s="1" t="s">
         <v>101</v>
       </c>
       <c r="G27" s="10"/>
@@ -3893,8 +4034,6 @@
       </c>
       <c r="C28" s="10"/>
       <c r="D28" s="11"/>
-      <c r="E28" s="39"/>
-      <c r="F28" s="39"/>
       <c r="G28" s="10"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
@@ -3904,7 +4043,6 @@
       <c r="B29" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C29" s="39"/>
       <c r="D29" s="24"/>
       <c r="E29" s="8"/>
       <c r="F29" s="8"/>
@@ -3918,17 +4056,16 @@
       <c r="B30" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C30" s="39"/>
       <c r="D30" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="E30" s="39" t="s">
+      <c r="E30" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="F30" s="39" t="s">
+      <c r="F30" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="G30" s="39" t="s">
+      <c r="G30" s="1" t="s">
         <v>105</v>
       </c>
       <c r="H30" s="10"/>
@@ -3940,17 +4077,16 @@
       <c r="B31" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C31" s="39"/>
       <c r="D31" s="11">
         <v>0</v>
       </c>
-      <c r="E31" s="39">
+      <c r="E31" s="1">
         <v>1.754</v>
       </c>
-      <c r="F31" s="39">
+      <c r="F31" s="1">
         <v>200</v>
       </c>
-      <c r="G31" s="39">
+      <c r="G31" s="1">
         <v>2500</v>
       </c>
       <c r="H31" s="10"/>
@@ -3962,17 +4098,16 @@
       <c r="B32" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C32" s="39"/>
       <c r="D32" s="11">
         <v>2.5</v>
       </c>
-      <c r="E32" s="39">
+      <c r="E32" s="1">
         <v>1.778</v>
       </c>
-      <c r="F32" s="39">
+      <c r="F32" s="1">
         <v>1250</v>
       </c>
-      <c r="G32" s="39">
+      <c r="G32" s="1">
         <v>1960</v>
       </c>
       <c r="H32" s="10"/>
@@ -3984,13 +4119,13 @@
       <c r="D33" s="11">
         <v>5</v>
       </c>
-      <c r="E33" s="39">
+      <c r="E33" s="1">
         <v>1.738</v>
       </c>
-      <c r="F33" s="39">
+      <c r="F33" s="1">
         <v>1000</v>
       </c>
-      <c r="G33" s="39">
+      <c r="G33" s="1">
         <v>2400</v>
       </c>
       <c r="H33" s="10"/>
@@ -3999,13 +4134,13 @@
       <c r="D34" s="11">
         <v>7.5</v>
       </c>
-      <c r="E34" s="39">
+      <c r="E34" s="1">
         <v>1.75</v>
       </c>
-      <c r="F34" s="39">
+      <c r="F34" s="1">
         <v>750</v>
       </c>
-      <c r="G34" s="39">
+      <c r="G34" s="1">
         <v>1900</v>
       </c>
       <c r="H34" s="10"/>
@@ -4014,13 +4149,13 @@
       <c r="D35" s="11">
         <v>10</v>
       </c>
-      <c r="E35" s="39">
+      <c r="E35" s="1">
         <v>1.754</v>
       </c>
-      <c r="F35" s="39">
+      <c r="F35" s="1">
         <v>450</v>
       </c>
-      <c r="G35" s="39">
+      <c r="G35" s="1">
         <v>1300</v>
       </c>
       <c r="H35" s="10"/>
@@ -4040,12 +4175,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="40c2d214-4ca5-4604-be72-e6c4439e5276">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="581c75f3-c23e-4d61-ac2d-458e1df0a137" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4256,41 +4393,54 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="40c2d214-4ca5-4604-be72-e6c4439e5276">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="581c75f3-c23e-4d61-ac2d-458e1df0a137" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F17E70AE-5CD9-46AD-9CD7-253B7D5337F5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="40c2d214-4ca5-4604-be72-e6c4439e5276"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="581c75f3-c23e-4d61-ac2d-458e1df0a137"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{548D2A98-E4BA-493B-BDDF-E4239C4502BF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="40c2d214-4ca5-4604-be72-e6c4439e5276"/>
+    <ds:schemaRef ds:uri="581c75f3-c23e-4d61-ac2d-458e1df0a137"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77CBFA7D-3A0A-48A4-8B12-895234E5D6E5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{548D2A98-E4BA-493B-BDDF-E4239C4502BF}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F17E70AE-5CD9-46AD-9CD7-253B7D5337F5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="581c75f3-c23e-4d61-ac2d-458e1df0a137"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="40c2d214-4ca5-4604-be72-e6c4439e5276"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added relevance to lit review and updated conclusion formatting
</commit_message>
<xml_diff>
--- a/Thesis Charts and Graphs.xlsx
+++ b/Thesis Charts and Graphs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://buckeyemailosu.sharepoint.com/sites/Tumortrackingresearch/Shared Documents/General/Theses/Isaac/Master's Thesis/ohio-state-coe-dissertation-template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="220" documentId="14_{BDDE5BD9-9B9B-1147-BD62-444B36ECC1DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6ADE7D6F-6544-AE49-9E4F-9DD574D2020B}"/>
+  <xr:revisionPtr revIDLastSave="290" documentId="14_{BDDE5BD9-9B9B-1147-BD62-444B36ECC1DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1324C56A-AC68-3047-85B3-D595D04AC406}"/>
   <bookViews>
-    <workbookView xWindow="980" yWindow="500" windowWidth="34860" windowHeight="21900" activeTab="2" xr2:uid="{16E6A821-3DC4-194B-96AE-E7BDD0CEA9F6}"/>
+    <workbookView xWindow="980" yWindow="500" windowWidth="34860" windowHeight="21900" activeTab="1" xr2:uid="{16E6A821-3DC4-194B-96AE-E7BDD0CEA9F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="155">
   <si>
     <t>Seroma Visibility (RefID 25)</t>
   </si>
@@ -430,20 +430,107 @@
 - Able to use existing gear and belt system for a more robust drive system</t>
   </si>
   <si>
-    <t>1, 2</t>
-  </si>
-  <si>
-    <t>3, 4</t>
-  </si>
-  <si>
-    <t>1, 7</t>
+    <t>Literature Review Section</t>
+  </si>
+  <si>
+    <t>sec:methodology:customerDiscovery</t>
+  </si>
+  <si>
+    <t>sec:literatureReview:currentMethods</t>
+  </si>
+  <si>
+    <t>sec:methodology:extrudingPLCL</t>
+  </si>
+  <si>
+    <t>sec:methodology:extrudingBaSO4</t>
+  </si>
+  <si>
+    <t>sec:literatureReview:extrusion</t>
+  </si>
+  <si>
+    <t>sec:literatureReview:extrusion:purging</t>
+  </si>
+  <si>
+    <t>sec:methodology:extrudingPLCL:purgingExtruder</t>
+  </si>
+  <si>
+    <t>sec:methodology:3dPrintingBaSO4</t>
+  </si>
+  <si>
+    <t>sec:literatureReview:printing</t>
+  </si>
+  <si>
+    <t>sec:methodology:effectsOfBaSO4:tensileTesting</t>
+  </si>
+  <si>
+    <t>sec:methodology:effectsOfBaSO4:flexuralTesting</t>
+  </si>
+  <si>
+    <t>sec:literatureReview:PLCL</t>
+  </si>
+  <si>
+    <t>sec:methodology:extrudingPLCL:pelletExtrusions:combiningMaterials</t>
+  </si>
+  <si>
+    <t>sec:methodology:3dPrintingPLCL</t>
+  </si>
+  <si>
+    <t>sec:literatureReview:alternativeDevices</t>
+  </si>
+  <si>
+    <t>sec:discussion:extrudingPLCL:powderExtrusion</t>
+  </si>
+  <si>
+    <t>sec:methodology:effectsOfBaSO4:imagingStudy</t>
+  </si>
+  <si>
+    <t>sec:literatureReview:radiopaque</t>
+  </si>
+  <si>
+    <t>sec:literatureReview:imaging</t>
+  </si>
+  <si>
+    <t>sec:literatureReview:materials</t>
+  </si>
+  <si>
+    <t>sec:methodology:effectsOfBaSO4</t>
+  </si>
+  <si>
+    <t>sec:literatureReview:testing</t>
+  </si>
+  <si>
+    <t>sec:results:effectsOfBaSO4:tensileTesting</t>
+  </si>
+  <si>
+    <t>sec:literatureReview:characterization</t>
+  </si>
+  <si>
+    <t>sec:methodology:materialCharacterization</t>
+  </si>
+  <si>
+    <t>sec:conclusion:futureWork:blendCharacterization</t>
+  </si>
+  <si>
+    <t>sec:conclusion:futureWork:testingPLCL</t>
+  </si>
+  <si>
+    <t>sec:literatureReview:roadmap</t>
+  </si>
+  <si>
+    <t>sec:methodology:starveFeeder:systemReDesign:beltTensioningPrototyping</t>
+  </si>
+  <si>
+    <t>sec:literatureReview:beltTension</t>
+  </si>
+  <si>
+    <t>Relevance in Thesis</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -464,6 +551,18 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFABB2BF"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFD19A66"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -739,7 +838,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -805,19 +904,22 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3290,10 +3392,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDAF9E8A-4B25-1B41-82F3-06803E42F3DE}">
-  <dimension ref="A1:L24"/>
+  <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="173" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19:J23"/>
+    <sheetView tabSelected="1" topLeftCell="F15" zoomScale="173" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19:H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3303,17 +3405,20 @@
     <col min="3" max="3" width="26.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="10.83203125" style="1"/>
+    <col min="6" max="6" width="10.83203125" style="1"/>
+    <col min="7" max="7" width="50.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="111" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.1640625" style="1" customWidth="1"/>
     <col min="10" max="10" width="10" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="70.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38"/>
+      <c r="B1" s="41"/>
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
       <c r="E1" s="8"/>
@@ -3416,7 +3521,8 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="11"/>
-      <c r="H9" s="10"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="9"/>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
@@ -3424,7 +3530,11 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="11"/>
+      <c r="G10" s="11"/>
       <c r="H10" s="10"/>
+      <c r="I10" s="42"/>
+      <c r="J10" s="42"/>
+      <c r="K10" s="42"/>
       <c r="L10" s="10"/>
     </row>
     <row r="11" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -3434,12 +3544,13 @@
       <c r="D11" s="13"/>
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
+      <c r="G11" s="12"/>
       <c r="H11" s="14"/>
-      <c r="J11" s="1" t="s">
+      <c r="I11" s="42"/>
+      <c r="J11" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="K11" s="42" t="s">
         <v>63</v>
       </c>
       <c r="L11" s="10" t="s">
@@ -3450,10 +3561,12 @@
       <c r="A12" s="11"/>
       <c r="E12" s="10"/>
       <c r="G12" s="11"/>
-      <c r="J12" s="1" t="s">
+      <c r="H12" s="42"/>
+      <c r="I12" s="42"/>
+      <c r="J12" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="K12" s="1" t="s">
+      <c r="K12" s="42" t="s">
         <v>65</v>
       </c>
       <c r="L12" s="10">
@@ -3475,10 +3588,12 @@
       </c>
       <c r="E13" s="10"/>
       <c r="G13" s="11"/>
-      <c r="J13" s="1" t="s">
+      <c r="H13" s="42"/>
+      <c r="I13" s="42"/>
+      <c r="J13" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="K13" s="1" t="s">
+      <c r="K13" s="42" t="s">
         <v>68</v>
       </c>
       <c r="L13" s="10">
@@ -3500,10 +3615,12 @@
       </c>
       <c r="E14" s="10"/>
       <c r="G14" s="11"/>
-      <c r="J14" s="1" t="s">
+      <c r="H14" s="42"/>
+      <c r="I14" s="42"/>
+      <c r="J14" s="42" t="s">
         <v>69</v>
       </c>
-      <c r="K14" s="1" t="s">
+      <c r="K14" s="42" t="s">
         <v>70</v>
       </c>
       <c r="L14" s="10">
@@ -3525,10 +3642,12 @@
       </c>
       <c r="E15" s="10"/>
       <c r="G15" s="11"/>
-      <c r="J15" s="1" t="s">
+      <c r="H15" s="42"/>
+      <c r="I15" s="42"/>
+      <c r="J15" s="42" t="s">
         <v>71</v>
       </c>
-      <c r="K15" s="1" t="s">
+      <c r="K15" s="42" t="s">
         <v>72</v>
       </c>
       <c r="L15" s="10">
@@ -3550,10 +3669,12 @@
       </c>
       <c r="E16" s="10"/>
       <c r="G16" s="11"/>
-      <c r="J16" s="1" t="s">
+      <c r="H16" s="42"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42" t="s">
         <v>73</v>
       </c>
-      <c r="K16" s="1" t="s">
+      <c r="K16" s="42" t="s">
         <v>74</v>
       </c>
       <c r="L16" s="10">
@@ -3576,10 +3697,10 @@
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="11"/>
       <c r="F18" s="10"/>
-      <c r="G18" s="24"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="9"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="34" t="s">
@@ -3598,7 +3719,13 @@
         <v>37</v>
       </c>
       <c r="F19" s="10"/>
-      <c r="G19" s="11"/>
+      <c r="G19" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="J19" s="42"/>
     </row>
     <row r="20" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A20" s="34" t="s">
@@ -3617,7 +3744,16 @@
         <v>41</v>
       </c>
       <c r="F20" s="10"/>
-      <c r="G20" s="11"/>
+      <c r="G20" s="44" t="s">
+        <v>125</v>
+      </c>
+      <c r="H20" s="1" t="str">
+        <f>_xlfn.TEXTJOIN("-"&amp;CHAR(10),TRUE,I20:N20)</f>
+        <v>sec:methodology:customerDiscovery</v>
+      </c>
+      <c r="I20" s="43" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="21" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="34" t="s">
@@ -3634,7 +3770,19 @@
         <v>46</v>
       </c>
       <c r="F21" s="10"/>
-      <c r="G21" s="11"/>
+      <c r="G21" s="44" t="s">
+        <v>128</v>
+      </c>
+      <c r="H21" s="1" t="str">
+        <f t="shared" ref="H21:H32" si="0">_xlfn.TEXTJOIN(",",TRUE,I21:N21)</f>
+        <v>sec:methodology:extrudingBaSO4,sec:methodology:extrudingPLCL</v>
+      </c>
+      <c r="I21" s="43" t="s">
+        <v>127</v>
+      </c>
+      <c r="J21" s="43" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="22" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="34" t="s">
@@ -3649,12 +3797,37 @@
         <v>45</v>
       </c>
       <c r="F22" s="10"/>
-      <c r="G22" s="11"/>
+      <c r="G22" s="44" t="s">
+        <v>129</v>
+      </c>
+      <c r="H22" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>sec:methodology:extrudingPLCL:purgingExtruder</v>
+      </c>
+      <c r="I22" s="43" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="11"/>
       <c r="F23" s="10"/>
-      <c r="G23" s="11"/>
+      <c r="G23" s="44" t="s">
+        <v>132</v>
+      </c>
+      <c r="H23" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>sec:methodology:3dPrintingBaSO4,sec:methodology:effectsOfBaSO4:tensileTesting,sec:methodology:effectsOfBaSO4:flexuralTesting</v>
+      </c>
+      <c r="I23" s="43" t="s">
+        <v>131</v>
+      </c>
+      <c r="J23" s="43" t="s">
+        <v>133</v>
+      </c>
+      <c r="K23" s="43" t="s">
+        <v>134</v>
+      </c>
+      <c r="L23" s="42"/>
     </row>
     <row r="24" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12"/>
@@ -3663,10 +3836,135 @@
       <c r="D24" s="13"/>
       <c r="E24" s="13"/>
       <c r="F24" s="14"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="14"/>
+      <c r="G24" s="44" t="s">
+        <v>135</v>
+      </c>
+      <c r="H24" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>sec:methodology:extrudingPLCL:pelletExtrusions:combiningMaterials,sec:methodology:3dPrintingPLCL</v>
+      </c>
+      <c r="I24" s="43" t="s">
+        <v>136</v>
+      </c>
+      <c r="J24" s="43" t="s">
+        <v>137</v>
+      </c>
+      <c r="K24" s="42"/>
+      <c r="L24" s="42"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G25" s="44" t="s">
+        <v>138</v>
+      </c>
+      <c r="H25" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>sec:discussion:extrudingPLCL:powderExtrusion</v>
+      </c>
+      <c r="I25" s="43" t="s">
+        <v>139</v>
+      </c>
+      <c r="J25" s="42"/>
+      <c r="K25" s="42"/>
+      <c r="L25" s="42"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G26" s="44" t="s">
+        <v>141</v>
+      </c>
+      <c r="H26" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>sec:methodology:extrudingBaSO4,sec:methodology:3dPrintingBaSO4,sec:methodology:effectsOfBaSO4:imagingStudy</v>
+      </c>
+      <c r="I26" s="43" t="s">
+        <v>127</v>
+      </c>
+      <c r="J26" s="43" t="s">
+        <v>131</v>
+      </c>
+      <c r="K26" s="43" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G27" s="44" t="s">
+        <v>142</v>
+      </c>
+      <c r="H27" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>sec:methodology:effectsOfBaSO4:imagingStudy</v>
+      </c>
+      <c r="I27" s="43" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G28" s="44" t="s">
+        <v>143</v>
+      </c>
+      <c r="H28" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>sec:methodology:effectsOfBaSO4,sec:conclusion:futureWork:testingPLCL</v>
+      </c>
+      <c r="I28" s="43" t="s">
+        <v>144</v>
+      </c>
+      <c r="J28" s="43" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G29" s="44" t="s">
+        <v>145</v>
+      </c>
+      <c r="H29" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>sec:results:effectsOfBaSO4:tensileTesting,sec:methodology:effectsOfBaSO4:flexuralTesting</v>
+      </c>
+      <c r="I29" s="43" t="s">
+        <v>146</v>
+      </c>
+      <c r="J29" s="43" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G30" s="44" t="s">
+        <v>147</v>
+      </c>
+      <c r="H30" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>sec:methodology:materialCharacterization,sec:conclusion:futureWork:blendCharacterization</v>
+      </c>
+      <c r="I30" s="43" t="s">
+        <v>148</v>
+      </c>
+      <c r="J30" s="43" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G31" s="44" t="s">
+        <v>151</v>
+      </c>
+      <c r="H31" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>sec:discussion:extrudingPLCL:powderExtrusion</v>
+      </c>
+      <c r="I31" s="43" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G32" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="H32" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>sec:methodology:starveFeeder:systemReDesign:beltTensioningPrototyping</v>
+      </c>
+      <c r="I32" s="43" t="s">
+        <v>152</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3679,10 +3977,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8738BA31-1A52-274A-92D6-B57235D8D2B5}">
-  <dimension ref="A1:M36"/>
+  <dimension ref="A1:O36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J5" zoomScale="238" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3695,7 +3993,7 @@
     <col min="13" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
         <v>75</v>
       </c>
@@ -3703,17 +4001,20 @@
         <v>76</v>
       </c>
       <c r="C1" s="9"/>
-      <c r="K1" s="1" t="s">
+      <c r="J1" s="24"/>
+      <c r="K1" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="8" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" ht="119" x14ac:dyDescent="0.2">
+      <c r="N1" s="8"/>
+      <c r="O1" s="9"/>
+    </row>
+    <row r="2" spans="1:15" ht="119" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>77</v>
       </c>
@@ -3721,17 +4022,16 @@
         <v>140</v>
       </c>
       <c r="C2" s="10"/>
-      <c r="K2" s="41" t="s">
+      <c r="J2" s="11"/>
+      <c r="K2" s="37" t="s">
         <v>109</v>
       </c>
-      <c r="L2" s="39" t="s">
+      <c r="L2" s="38" t="s">
         <v>110</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="O2" s="10"/>
+    </row>
+    <row r="3" spans="1:15" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>78</v>
       </c>
@@ -3739,17 +4039,16 @@
         <v>155</v>
       </c>
       <c r="C3" s="10"/>
-      <c r="K3" s="41" t="s">
+      <c r="J3" s="11"/>
+      <c r="K3" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="L3" s="40" t="s">
+      <c r="L3" s="39" t="s">
         <v>112</v>
       </c>
-      <c r="M3" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="O3" s="10"/>
+    </row>
+    <row r="4" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>79</v>
       </c>
@@ -3757,14 +4056,16 @@
         <v>160</v>
       </c>
       <c r="C4" s="10"/>
+      <c r="J4" s="11"/>
       <c r="K4" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="L4" s="39" t="s">
+      <c r="L4" s="38" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="O4" s="10"/>
+    </row>
+    <row r="5" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>80</v>
       </c>
@@ -3772,27 +4073,28 @@
         <v>160</v>
       </c>
       <c r="C5" s="10"/>
+      <c r="J5" s="11"/>
       <c r="K5" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="L5" s="39" t="s">
+      <c r="L5" s="38" t="s">
         <v>116</v>
       </c>
-      <c r="M5" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="O5" s="10"/>
+    </row>
+    <row r="6" spans="1:15" ht="52" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
       <c r="C6" s="10"/>
+      <c r="J6" s="11"/>
       <c r="K6" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="L6" s="39" t="s">
+      <c r="L6" s="38" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" ht="68" x14ac:dyDescent="0.2">
+      <c r="O6" s="10"/>
+    </row>
+    <row r="7" spans="1:15" ht="68" x14ac:dyDescent="0.2">
       <c r="A7" s="24"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
@@ -3801,42 +4103,47 @@
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
-      <c r="I7" s="9"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="11"/>
       <c r="K7" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="L7" s="39" t="s">
+      <c r="L7" s="38" t="s">
         <v>120</v>
       </c>
-      <c r="M7" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="136" x14ac:dyDescent="0.2">
+      <c r="O7" s="10"/>
+    </row>
+    <row r="8" spans="1:15" ht="136" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
         <v>81</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="I8" s="10"/>
+      <c r="J8" s="11"/>
       <c r="K8" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="L8" s="39" t="s">
+      <c r="L8" s="38" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O8" s="10"/>
+    </row>
+    <row r="9" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
         <v>60</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
       </c>
-      <c r="I9" s="10"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="J9" s="12"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="14"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="11">
         <v>70</v>
       </c>
@@ -3845,7 +4152,7 @@
       </c>
       <c r="I10" s="10"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="11">
         <v>80</v>
       </c>
@@ -3854,7 +4161,7 @@
       </c>
       <c r="I11" s="10"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
         <v>90</v>
       </c>
@@ -3863,7 +4170,7 @@
       </c>
       <c r="I12" s="10"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="11">
         <v>100</v>
       </c>
@@ -3872,7 +4179,7 @@
       </c>
       <c r="I13" s="10"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="11">
         <v>110</v>
       </c>
@@ -3881,7 +4188,7 @@
       </c>
       <c r="I14" s="10"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="11">
         <v>120</v>
       </c>
@@ -3890,7 +4197,7 @@
       </c>
       <c r="I15" s="10"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="11">
         <v>130</v>
       </c>
@@ -4175,19 +4482,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="40c2d214-4ca5-4604-be72-e6c4439e5276">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="581c75f3-c23e-4d61-ac2d-458e1df0a137" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010020A0C45D55D81B409E1ED58F2E9DADA4" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b3439157d04fb2c0c2146dbea8d1ca4f">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="40c2d214-4ca5-4604-be72-e6c4439e5276" xmlns:ns3="581c75f3-c23e-4d61-ac2d-458e1df0a137" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4c3248ab5c1b5bd60be37440245572d8" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010020A0C45D55D81B409E1ED58F2E9DADA4" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cbded72ff34985fcf4aed41856a1fc63">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="40c2d214-4ca5-4604-be72-e6c4439e5276" xmlns:ns3="581c75f3-c23e-4d61-ac2d-458e1df0a137" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1df4a492fd975042fd478bddf68f177e" ns2:_="" ns3:_="">
     <xsd:import namespace="40c2d214-4ca5-4604-be72-e6c4439e5276"/>
     <xsd:import namespace="581c75f3-c23e-4d61-ac2d-458e1df0a137"/>
     <xsd:element name="properties">
@@ -4208,6 +4513,7 @@
                 <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceBillingMetadata" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -4275,6 +4581,11 @@
     <xsd:element name="MediaLengthInSeconds" ma:index="20" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceBillingMetadata" ma:index="21" nillable="true" ma:displayName="MediaServiceBillingMetadata" ma:hidden="true" ma:internalName="MediaServiceBillingMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -4393,33 +4704,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="40c2d214-4ca5-4604-be72-e6c4439e5276">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="581c75f3-c23e-4d61-ac2d-458e1df0a137" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F17E70AE-5CD9-46AD-9CD7-253B7D5337F5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77CBFA7D-3A0A-48A4-8B12-895234E5D6E5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="40c2d214-4ca5-4604-be72-e6c4439e5276"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="581c75f3-c23e-4d61-ac2d-458e1df0a137"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{548D2A98-E4BA-493B-BDDF-E4239C4502BF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1DC16A6F-6309-4CD1-8C9A-754368374312}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
@@ -4438,9 +4742,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77CBFA7D-3A0A-48A4-8B12-895234E5D6E5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F17E70AE-5CD9-46AD-9CD7-253B7D5337F5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="581c75f3-c23e-4d61-ac2d-458e1df0a137"/>
+    <ds:schemaRef ds:uri="40c2d214-4ca5-4604-be72-e6c4439e5276"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Adding thesis committee additions
</commit_message>
<xml_diff>
--- a/Thesis Charts and Graphs.xlsx
+++ b/Thesis Charts and Graphs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://buckeyemailosu.sharepoint.com/sites/Tumortrackingresearch/Shared Documents/General/Theses/Isaac/Master's Thesis/ohio-state-coe-dissertation-template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="611" documentId="14_{BDDE5BD9-9B9B-1147-BD62-444B36ECC1DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DEB528F8-B69F-4346-B8AE-A6CF64A1D01C}"/>
+  <xr:revisionPtr revIDLastSave="779" documentId="14_{BDDE5BD9-9B9B-1147-BD62-444B36ECC1DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{350FC18D-BB89-F648-9ED0-F823F57C9F1B}"/>
   <bookViews>
     <workbookView xWindow="980" yWindow="500" windowWidth="34860" windowHeight="21900" activeTab="4" xr2:uid="{16E6A821-3DC4-194B-96AE-E7BDD0CEA9F6}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="208">
   <si>
     <t>Seroma Visibility (RefID 25)</t>
   </si>
@@ -626,6 +626,87 @@
   </si>
   <si>
     <t>Submitted Final Thesis</t>
+  </si>
+  <si>
+    <t>1,2</t>
+  </si>
+  <si>
+    <t>19,23</t>
+  </si>
+  <si>
+    <t>3,6</t>
+  </si>
+  <si>
+    <t>7,8,9,10</t>
+  </si>
+  <si>
+    <t>6,11</t>
+  </si>
+  <si>
+    <t>8,12,13</t>
+  </si>
+  <si>
+    <t>6,12,16,17</t>
+  </si>
+  <si>
+    <t>6,12,14,15</t>
+  </si>
+  <si>
+    <t>6,12,18</t>
+  </si>
+  <si>
+    <t>24,53</t>
+  </si>
+  <si>
+    <t>6,19</t>
+  </si>
+  <si>
+    <t>6,20</t>
+  </si>
+  <si>
+    <t>6,19,21,22</t>
+  </si>
+  <si>
+    <t>19,26</t>
+  </si>
+  <si>
+    <t>19,27</t>
+  </si>
+  <si>
+    <t>28,29</t>
+  </si>
+  <si>
+    <t>25,32,33,34,35,36</t>
+  </si>
+  <si>
+    <t>38,39</t>
+  </si>
+  <si>
+    <t>30,44,45</t>
+  </si>
+  <si>
+    <t>45,46</t>
+  </si>
+  <si>
+    <t>4,5</t>
+  </si>
+  <si>
+    <t>40,41,42,43</t>
+  </si>
+  <si>
+    <t>44,50</t>
+  </si>
+  <si>
+    <t>45,51</t>
+  </si>
+  <si>
+    <t>Slide Number</t>
+  </si>
+  <si>
+    <t>Citations On Slide</t>
+  </si>
+  <si>
+    <t>Latex Compatible</t>
   </si>
 </sst>
 </file>
@@ -1172,7 +1253,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -1186,6 +1267,9 @@
           <bgColor theme="5" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3251,12 +3335,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{050E9A4A-8293-BB40-9CD7-F1E552DAE50F}" name="Table1" displayName="Table1" ref="A1:C47" totalsRowShown="0">
-  <autoFilter ref="A1:C47" xr:uid="{050E9A4A-8293-BB40-9CD7-F1E552DAE50F}"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{050E9A4A-8293-BB40-9CD7-F1E552DAE50F}" name="Table1" displayName="Table1" ref="A1:D55" totalsRowShown="0">
+  <autoFilter ref="A1:D55" xr:uid="{050E9A4A-8293-BB40-9CD7-F1E552DAE50F}"/>
+  <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{44529169-2D49-F44B-B04F-E665873864EA}" name="In-Slide Citation Number"/>
     <tableColumn id="2" xr3:uid="{72E4E51F-F402-C347-9896-3BD0D1A4ECA5}" name="RefID"/>
     <tableColumn id="3" xr3:uid="{DE08DEAE-4261-FF48-8826-9474B4ACAB10}" name="Number in Thesis"/>
+    <tableColumn id="4" xr3:uid="{D4ED6B48-629F-5B40-8062-19F778D0143B}" name="Latex Compatible" dataDxfId="2">
+      <calculatedColumnFormula>"\cite{RefWorks:"&amp;B2&amp;"}"</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4949,10 +5036,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC3402C8-0B15-1042-9A3C-23E5711B1B4C}">
-  <dimension ref="A1:I48"/>
+  <dimension ref="A1:K64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4960,13 +5047,14 @@
     <col min="1" max="1" width="24.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="17.83203125" customWidth="1"/>
+    <col min="7" max="7" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>166</v>
       </c>
@@ -4976,20 +5064,23 @@
       <c r="C1" t="s">
         <v>167</v>
       </c>
-      <c r="E1" s="47" t="s">
+      <c r="D1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G1" s="47" t="s">
         <v>165</v>
       </c>
-      <c r="F1" s="47" t="s">
+      <c r="H1" s="47" t="s">
         <v>168</v>
       </c>
-      <c r="H1" s="50" t="s">
+      <c r="J1" s="50" t="s">
         <v>168</v>
       </c>
-      <c r="I1" s="48">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K1" s="48">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4999,23 +5090,27 @@
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="E2" cm="1">
-        <f t="array" ref="E2:E48">_xlfn.UNIQUE(B2:B500)</f>
+      <c r="D2" t="str">
+        <f t="shared" ref="D2:D33" si="0">"\cite{RefWorks:"&amp;B2&amp;"}"</f>
+        <v>\cite{RefWorks:36}</v>
+      </c>
+      <c r="G2" cm="1">
+        <f t="array" ref="G2:G56">_xlfn.UNIQUE(B2:B500)</f>
         <v>36</v>
       </c>
-      <c r="F2">
-        <f>IFERROR(VLOOKUP(E2,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
+      <c r="H2">
+        <f>IFERROR(VLOOKUP(G2,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
         <v>1</v>
       </c>
-      <c r="H2" s="51" t="s">
+      <c r="J2" s="51" t="s">
         <v>169</v>
       </c>
-      <c r="I2" s="49">
-        <f>IFERROR(INDEX(Table1[In-Slide Citation Number],MATCH(I1,Table1[Number in Thesis],0)),"Reference Not Used Yet!")</f>
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K2" s="49" t="str">
+        <f>IFERROR(INDEX(Table1[In-Slide Citation Number],MATCH(K1,Table1[Number in Thesis],0)),"Reference Not Used Yet!")</f>
+        <v>Reference Not Used Yet!</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -5025,15 +5120,19 @@
       <c r="C3">
         <v>2</v>
       </c>
-      <c r="E3">
+      <c r="D3" t="str">
+        <f t="shared" si="0"/>
+        <v>\cite{RefWorks:150}</v>
+      </c>
+      <c r="G3">
         <v>150</v>
       </c>
-      <c r="F3">
-        <f>IFERROR(VLOOKUP(E3,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
+      <c r="H3">
+        <f>IFERROR(VLOOKUP(G3,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -5043,15 +5142,25 @@
       <c r="C4">
         <v>20</v>
       </c>
-      <c r="E4">
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>\cite{RefWorks:37}</v>
+      </c>
+      <c r="G4">
         <v>37</v>
       </c>
-      <c r="F4">
-        <f>IFERROR(VLOOKUP(E4,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
+      <c r="H4">
+        <f>IFERROR(VLOOKUP(G4,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J4" t="s">
+        <v>205</v>
+      </c>
+      <c r="K4" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -5061,15 +5170,25 @@
       <c r="C5">
         <v>12</v>
       </c>
-      <c r="E5">
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>\cite{RefWorks:151}</v>
+      </c>
+      <c r="G5">
         <v>151</v>
       </c>
-      <c r="F5">
-        <f>IFERROR(VLOOKUP(E5,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
+      <c r="H5">
+        <f>IFERROR(VLOOKUP(G5,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J5">
+        <v>6</v>
+      </c>
+      <c r="K5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -5079,15 +5198,25 @@
       <c r="C6">
         <v>13</v>
       </c>
-      <c r="E6">
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>\cite{RefWorks:365}</v>
+      </c>
+      <c r="G6">
         <v>365</v>
       </c>
-      <c r="F6">
-        <f>IFERROR(VLOOKUP(E6,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
+      <c r="H6">
+        <f>IFERROR(VLOOKUP(G6,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J6">
+        <v>7</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -5097,15 +5226,25 @@
       <c r="C7">
         <v>11</v>
       </c>
-      <c r="E7">
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>\cite{RefWorks:370}</v>
+      </c>
+      <c r="G7">
         <v>370</v>
       </c>
-      <c r="F7">
-        <f>IFERROR(VLOOKUP(E7,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
+      <c r="H7">
+        <f>IFERROR(VLOOKUP(G7,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J7">
+        <v>8</v>
+      </c>
+      <c r="K7" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -5115,15 +5254,25 @@
       <c r="C8">
         <v>5</v>
       </c>
-      <c r="E8">
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>\cite{RefWorks:157}</v>
+      </c>
+      <c r="G8">
         <v>157</v>
       </c>
-      <c r="F8">
-        <f>IFERROR(VLOOKUP(E8,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
+      <c r="H8">
+        <f>IFERROR(VLOOKUP(G8,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J8">
+        <v>9</v>
+      </c>
+      <c r="K8" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -5133,15 +5282,25 @@
       <c r="C9">
         <v>6</v>
       </c>
-      <c r="E9">
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v>\cite{RefWorks:198}</v>
+      </c>
+      <c r="G9">
         <v>198</v>
       </c>
-      <c r="F9">
-        <f>IFERROR(VLOOKUP(E9,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
+      <c r="H9">
+        <f>IFERROR(VLOOKUP(G9,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J9">
+        <v>10</v>
+      </c>
+      <c r="K9" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -5151,30 +5310,50 @@
       <c r="C10">
         <v>7</v>
       </c>
-      <c r="E10">
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v>\cite{RefWorks:375}</v>
+      </c>
+      <c r="G10">
         <v>375</v>
       </c>
-      <c r="F10">
-        <f>IFERROR(VLOOKUP(E10,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
+      <c r="H10">
+        <f>IFERROR(VLOOKUP(G10,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J10">
+        <v>11</v>
+      </c>
+      <c r="K10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
         <v>503</v>
       </c>
-      <c r="E11">
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v>\cite{RefWorks:503}</v>
+      </c>
+      <c r="G11">
         <v>503</v>
       </c>
-      <c r="F11">
-        <f>IFERROR(VLOOKUP(E11,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
+      <c r="H11">
+        <f>IFERROR(VLOOKUP(G11,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J11">
+        <v>12</v>
+      </c>
+      <c r="K11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -5184,15 +5363,25 @@
       <c r="C12">
         <v>21</v>
       </c>
-      <c r="E12">
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v>\cite{RefWorks:38}</v>
+      </c>
+      <c r="G12">
         <v>38</v>
       </c>
-      <c r="F12">
-        <f>IFERROR(VLOOKUP(E12,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
+      <c r="H12">
+        <f>IFERROR(VLOOKUP(G12,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
         <v>21</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J12">
+        <v>13</v>
+      </c>
+      <c r="K12" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -5202,15 +5391,25 @@
       <c r="C13">
         <v>8</v>
       </c>
-      <c r="E13">
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v>\cite{RefWorks:25}</v>
+      </c>
+      <c r="G13">
         <v>25</v>
       </c>
-      <c r="F13">
-        <f>IFERROR(VLOOKUP(E13,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
+      <c r="H13">
+        <f>IFERROR(VLOOKUP(G13,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
         <v>8</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J13">
+        <v>15</v>
+      </c>
+      <c r="K13" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -5220,45 +5419,75 @@
       <c r="C14">
         <v>77</v>
       </c>
-      <c r="E14">
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v>\cite{RefWorks:197}</v>
+      </c>
+      <c r="G14">
         <v>197</v>
       </c>
-      <c r="F14">
-        <f>IFERROR(VLOOKUP(E14,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
+      <c r="H14">
+        <f>IFERROR(VLOOKUP(G14,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
         <v>77</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J14">
+        <v>16</v>
+      </c>
+      <c r="K14" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15">
         <v>39</v>
       </c>
-      <c r="E15">
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v>\cite{RefWorks:39}</v>
+      </c>
+      <c r="G15">
         <v>39</v>
       </c>
-      <c r="F15">
-        <f>IFERROR(VLOOKUP(E15,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
+      <c r="H15">
+        <f>IFERROR(VLOOKUP(G15,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J15">
+        <v>17</v>
+      </c>
+      <c r="K15" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16">
         <v>49</v>
       </c>
-      <c r="E16">
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v>\cite{RefWorks:49}</v>
+      </c>
+      <c r="G16">
         <v>49</v>
       </c>
-      <c r="F16">
-        <f>IFERROR(VLOOKUP(E16,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
+      <c r="H16">
+        <f>IFERROR(VLOOKUP(G16,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J16">
+        <v>18</v>
+      </c>
+      <c r="K16" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -5268,30 +5497,50 @@
       <c r="C17">
         <v>90</v>
       </c>
-      <c r="E17">
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v>\cite{RefWorks:28}</v>
+      </c>
+      <c r="G17">
         <v>28</v>
       </c>
-      <c r="F17">
-        <f>IFERROR(VLOOKUP(E17,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
+      <c r="H17">
+        <f>IFERROR(VLOOKUP(G17,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
         <v>90</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J17">
+        <v>19</v>
+      </c>
+      <c r="K17" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18">
         <v>50</v>
       </c>
-      <c r="E18">
+      <c r="D18" t="str">
+        <f t="shared" si="0"/>
+        <v>\cite{RefWorks:50}</v>
+      </c>
+      <c r="G18">
         <v>50</v>
       </c>
-      <c r="F18">
-        <f>IFERROR(VLOOKUP(E18,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
+      <c r="H18">
+        <f>IFERROR(VLOOKUP(G18,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J18">
+        <v>20</v>
+      </c>
+      <c r="K18" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -5301,15 +5550,25 @@
       <c r="C19">
         <v>25</v>
       </c>
-      <c r="E19">
+      <c r="D19" t="str">
+        <f t="shared" si="0"/>
+        <v>\cite{RefWorks:191}</v>
+      </c>
+      <c r="G19">
         <v>191</v>
       </c>
-      <c r="F19">
-        <f>IFERROR(VLOOKUP(E19,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
+      <c r="H19">
+        <f>IFERROR(VLOOKUP(G19,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
         <v>25</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J19">
+        <v>21</v>
+      </c>
+      <c r="K19" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -5319,30 +5578,50 @@
       <c r="C20">
         <v>9</v>
       </c>
-      <c r="E20">
+      <c r="D20" t="str">
+        <f t="shared" si="0"/>
+        <v>\cite{RefWorks:371}</v>
+      </c>
+      <c r="G20">
         <v>371</v>
       </c>
-      <c r="F20">
-        <f>IFERROR(VLOOKUP(E20,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
+      <c r="H20">
+        <f>IFERROR(VLOOKUP(G20,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
         <v>9</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J20">
+        <v>22</v>
+      </c>
+      <c r="K20" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21">
         <v>52</v>
       </c>
-      <c r="E21">
+      <c r="D21" t="str">
+        <f t="shared" si="0"/>
+        <v>\cite{RefWorks:52}</v>
+      </c>
+      <c r="G21">
         <v>52</v>
       </c>
-      <c r="F21">
-        <f>IFERROR(VLOOKUP(E21,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
+      <c r="H21">
+        <f>IFERROR(VLOOKUP(G21,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J21">
+        <v>23</v>
+      </c>
+      <c r="K21" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -5352,15 +5631,25 @@
       <c r="C22">
         <v>10</v>
       </c>
-      <c r="E22">
+      <c r="D22" t="str">
+        <f t="shared" si="0"/>
+        <v>\cite{RefWorks:372}</v>
+      </c>
+      <c r="G22">
         <v>372</v>
       </c>
-      <c r="F22">
-        <f>IFERROR(VLOOKUP(E22,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
+      <c r="H22">
+        <f>IFERROR(VLOOKUP(G22,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
         <v>10</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J22">
+        <v>24</v>
+      </c>
+      <c r="K22" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -5370,30 +5659,50 @@
       <c r="C23">
         <v>23</v>
       </c>
-      <c r="E23">
+      <c r="D23" t="str">
+        <f t="shared" si="0"/>
+        <v>\cite{RefWorks:47}</v>
+      </c>
+      <c r="G23">
         <v>47</v>
       </c>
-      <c r="F23">
-        <f>IFERROR(VLOOKUP(E23,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
+      <c r="H23">
+        <f>IFERROR(VLOOKUP(G23,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
         <v>23</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J23">
+        <v>27</v>
+      </c>
+      <c r="K23" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24">
         <v>338</v>
       </c>
-      <c r="E24">
+      <c r="D24" t="str">
+        <f t="shared" si="0"/>
+        <v>\cite{RefWorks:338}</v>
+      </c>
+      <c r="G24">
         <v>338</v>
       </c>
-      <c r="F24">
-        <f>IFERROR(VLOOKUP(E24,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
+      <c r="H24">
+        <f>IFERROR(VLOOKUP(G24,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J24">
+        <v>29</v>
+      </c>
+      <c r="K24">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -5403,30 +5712,50 @@
       <c r="C25">
         <v>26</v>
       </c>
-      <c r="E25">
+      <c r="D25" t="str">
+        <f t="shared" si="0"/>
+        <v>\cite{RefWorks:344}</v>
+      </c>
+      <c r="G25">
         <v>344</v>
       </c>
-      <c r="F25">
-        <f>IFERROR(VLOOKUP(E25,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
+      <c r="H25">
+        <f>IFERROR(VLOOKUP(G25,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
         <v>26</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J25">
+        <v>30</v>
+      </c>
+      <c r="K25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26">
         <v>504</v>
       </c>
-      <c r="E26">
+      <c r="D26" t="str">
+        <f t="shared" si="0"/>
+        <v>\cite{RefWorks:504}</v>
+      </c>
+      <c r="G26">
         <v>504</v>
       </c>
-      <c r="F26">
-        <f>IFERROR(VLOOKUP(E26,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
+      <c r="H26">
+        <f>IFERROR(VLOOKUP(G26,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J26">
+        <v>31</v>
+      </c>
+      <c r="K26">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -5436,15 +5765,25 @@
       <c r="C27">
         <v>84</v>
       </c>
-      <c r="E27">
+      <c r="D27" t="str">
+        <f t="shared" si="0"/>
+        <v>\cite{RefWorks:387}</v>
+      </c>
+      <c r="G27">
         <v>387</v>
       </c>
-      <c r="F27">
-        <f>IFERROR(VLOOKUP(E27,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
+      <c r="H27">
+        <f>IFERROR(VLOOKUP(G27,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
         <v>84</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J27">
+        <v>32</v>
+      </c>
+      <c r="K27" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -5454,15 +5793,25 @@
       <c r="C28">
         <v>83</v>
       </c>
-      <c r="E28">
+      <c r="D28" t="str">
+        <f t="shared" si="0"/>
+        <v>\cite{RefWorks:204}</v>
+      </c>
+      <c r="G28">
         <v>204</v>
       </c>
-      <c r="F28">
-        <f>IFERROR(VLOOKUP(E28,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
+      <c r="H28">
+        <f>IFERROR(VLOOKUP(G28,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
         <v>83</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J28">
+        <v>33</v>
+      </c>
+      <c r="K28">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -5472,15 +5821,25 @@
       <c r="C29">
         <v>28</v>
       </c>
-      <c r="E29">
+      <c r="D29" t="str">
+        <f t="shared" si="0"/>
+        <v>\cite{RefWorks:266}</v>
+      </c>
+      <c r="G29">
         <v>266</v>
       </c>
-      <c r="F29">
-        <f>IFERROR(VLOOKUP(E29,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
+      <c r="H29">
+        <f>IFERROR(VLOOKUP(G29,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J29">
+        <v>34</v>
+      </c>
+      <c r="K29">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -5490,15 +5849,25 @@
       <c r="C30">
         <v>29</v>
       </c>
-      <c r="E30">
+      <c r="D30" t="str">
+        <f t="shared" si="0"/>
+        <v>\cite{RefWorks:309}</v>
+      </c>
+      <c r="G30">
         <v>309</v>
       </c>
-      <c r="F30">
-        <f>IFERROR(VLOOKUP(E30,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
+      <c r="H30">
+        <f>IFERROR(VLOOKUP(G30,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J30">
+        <v>35</v>
+      </c>
+      <c r="K30">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -5508,15 +5877,25 @@
       <c r="C31">
         <v>33</v>
       </c>
-      <c r="E31">
+      <c r="D31" t="str">
+        <f t="shared" si="0"/>
+        <v>\cite{RefWorks:396}</v>
+      </c>
+      <c r="G31">
         <v>396</v>
       </c>
-      <c r="F31">
-        <f>IFERROR(VLOOKUP(E31,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
+      <c r="H31">
+        <f>IFERROR(VLOOKUP(G31,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
         <v>33</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J31">
+        <v>36</v>
+      </c>
+      <c r="K31" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -5526,15 +5905,25 @@
       <c r="C32">
         <v>34</v>
       </c>
-      <c r="E32">
+      <c r="D32" t="str">
+        <f t="shared" si="0"/>
+        <v>\cite{RefWorks:393}</v>
+      </c>
+      <c r="G32">
         <v>393</v>
       </c>
-      <c r="F32">
-        <f>IFERROR(VLOOKUP(E32,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
+      <c r="H32">
+        <f>IFERROR(VLOOKUP(G32,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
         <v>34</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J32">
+        <v>38</v>
+      </c>
+      <c r="K32">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -5544,15 +5933,25 @@
       <c r="C33">
         <v>64</v>
       </c>
-      <c r="E33">
+      <c r="D33" t="str">
+        <f t="shared" si="0"/>
+        <v>\cite{RefWorks:482}</v>
+      </c>
+      <c r="G33">
         <v>482</v>
       </c>
-      <c r="F33">
-        <f>IFERROR(VLOOKUP(E33,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
+      <c r="H33">
+        <f>IFERROR(VLOOKUP(G33,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
         <v>64</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J33">
+        <v>39</v>
+      </c>
+      <c r="K33">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -5562,15 +5961,25 @@
       <c r="C34">
         <v>65</v>
       </c>
-      <c r="E34">
+      <c r="D34" t="str">
+        <f t="shared" ref="D34:D55" si="1">"\cite{RefWorks:"&amp;B34&amp;"}"</f>
+        <v>\cite{RefWorks:483}</v>
+      </c>
+      <c r="G34">
         <v>483</v>
       </c>
-      <c r="F34">
-        <f>IFERROR(VLOOKUP(E34,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
+      <c r="H34">
+        <f>IFERROR(VLOOKUP(G34,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
         <v>65</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J34">
+        <v>40</v>
+      </c>
+      <c r="K34">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -5580,15 +5989,25 @@
       <c r="C35">
         <v>66</v>
       </c>
-      <c r="E35">
+      <c r="D35" t="str">
+        <f t="shared" si="1"/>
+        <v>\cite{RefWorks:484}</v>
+      </c>
+      <c r="G35">
         <v>484</v>
       </c>
-      <c r="F35">
-        <f>IFERROR(VLOOKUP(E35,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
+      <c r="H35">
+        <f>IFERROR(VLOOKUP(G35,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
         <v>66</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J35">
+        <v>41</v>
+      </c>
+      <c r="K35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -5598,15 +6017,25 @@
       <c r="C36">
         <v>67</v>
       </c>
-      <c r="E36">
+      <c r="D36" t="str">
+        <f t="shared" si="1"/>
+        <v>\cite{RefWorks:485}</v>
+      </c>
+      <c r="G36">
         <v>485</v>
       </c>
-      <c r="F36">
-        <f>IFERROR(VLOOKUP(E36,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
+      <c r="H36">
+        <f>IFERROR(VLOOKUP(G36,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
         <v>67</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J36">
+        <v>42</v>
+      </c>
+      <c r="K36">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -5616,15 +6045,25 @@
       <c r="C37">
         <v>68</v>
       </c>
-      <c r="E37">
+      <c r="D37" t="str">
+        <f t="shared" si="1"/>
+        <v>\cite{RefWorks:486}</v>
+      </c>
+      <c r="G37">
         <v>486</v>
       </c>
-      <c r="F37">
-        <f>IFERROR(VLOOKUP(E37,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
+      <c r="H37">
+        <f>IFERROR(VLOOKUP(G37,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
         <v>68</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J37">
+        <v>43</v>
+      </c>
+      <c r="K37">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -5634,15 +6073,25 @@
       <c r="C38">
         <v>117</v>
       </c>
-      <c r="E38">
+      <c r="D38" t="str">
+        <f t="shared" si="1"/>
+        <v>\cite{RefWorks:255}</v>
+      </c>
+      <c r="G38">
         <v>255</v>
       </c>
-      <c r="F38">
-        <f>IFERROR(VLOOKUP(E38,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
+      <c r="H38">
+        <f>IFERROR(VLOOKUP(G38,Table1[[RefID]:[Number in Thesis]],2,0),"")</f>
         <v>117</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J38">
+        <v>45</v>
+      </c>
+      <c r="K38" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -5652,11 +6101,21 @@
       <c r="C39">
         <v>74</v>
       </c>
-      <c r="E39">
+      <c r="D39" t="str">
+        <f t="shared" si="1"/>
+        <v>\cite{RefWorks:490}</v>
+      </c>
+      <c r="G39">
         <v>490</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J39">
+        <v>50</v>
+      </c>
+      <c r="K39" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -5666,11 +6125,21 @@
       <c r="C40">
         <v>75</v>
       </c>
-      <c r="E40">
+      <c r="D40" t="str">
+        <f t="shared" si="1"/>
+        <v>\cite{RefWorks:491}</v>
+      </c>
+      <c r="G40">
         <v>491</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J40">
+        <v>51</v>
+      </c>
+      <c r="K40">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -5680,11 +6149,21 @@
       <c r="C41">
         <v>70</v>
       </c>
-      <c r="E41">
+      <c r="D41" t="str">
+        <f t="shared" si="1"/>
+        <v>\cite{RefWorks:496}</v>
+      </c>
+      <c r="G41">
         <v>496</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J41">
+        <v>53</v>
+      </c>
+      <c r="K41">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -5694,11 +6173,21 @@
       <c r="C42">
         <v>71</v>
       </c>
-      <c r="E42">
+      <c r="D42" t="str">
+        <f t="shared" si="1"/>
+        <v>\cite{RefWorks:497}</v>
+      </c>
+      <c r="G42">
         <v>497</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J42">
+        <v>54</v>
+      </c>
+      <c r="K42">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -5708,11 +6197,21 @@
       <c r="C43">
         <v>72</v>
       </c>
-      <c r="E43">
+      <c r="D43" t="str">
+        <f t="shared" si="1"/>
+        <v>\cite{RefWorks:498}</v>
+      </c>
+      <c r="G43">
         <v>498</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J43">
+        <v>55</v>
+      </c>
+      <c r="K43">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -5722,11 +6221,21 @@
       <c r="C44">
         <v>73</v>
       </c>
-      <c r="E44">
+      <c r="D44" t="str">
+        <f t="shared" si="1"/>
+        <v>\cite{RefWorks:499}</v>
+      </c>
+      <c r="G44">
         <v>499</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J44">
+        <v>56</v>
+      </c>
+      <c r="K44">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -5736,11 +6245,21 @@
       <c r="C45">
         <v>118</v>
       </c>
-      <c r="E45">
+      <c r="D45" t="str">
+        <f t="shared" si="1"/>
+        <v>\cite{RefWorks:62}</v>
+      </c>
+      <c r="G45">
         <v>62</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J45">
+        <v>58</v>
+      </c>
+      <c r="K45" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -5750,11 +6269,21 @@
       <c r="C46">
         <v>124</v>
       </c>
-      <c r="E46">
+      <c r="D46" t="str">
+        <f t="shared" si="1"/>
+        <v>\cite{RefWorks:77}</v>
+      </c>
+      <c r="G46">
         <v>77</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J46">
+        <v>59</v>
+      </c>
+      <c r="K46">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -5764,27 +6293,294 @@
       <c r="C47">
         <v>127</v>
       </c>
-      <c r="E47">
+      <c r="D47" t="str">
+        <f t="shared" si="1"/>
+        <v>\cite{RefWorks:78}</v>
+      </c>
+      <c r="G47">
         <v>78</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="E48">
+      <c r="J47">
+        <v>66</v>
+      </c>
+      <c r="K47" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48">
+        <v>4</v>
+      </c>
+      <c r="C48">
+        <v>85</v>
+      </c>
+      <c r="D48" t="str">
+        <f t="shared" si="1"/>
+        <v>\cite{RefWorks:4}</v>
+      </c>
+      <c r="G48">
+        <v>4</v>
+      </c>
+      <c r="J48">
+        <v>84</v>
+      </c>
+      <c r="K48">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49">
+        <v>33</v>
+      </c>
+      <c r="C49">
+        <v>39</v>
+      </c>
+      <c r="D49" t="str">
+        <f t="shared" si="1"/>
+        <v>\cite{RefWorks:33}</v>
+      </c>
+      <c r="G49">
+        <v>33</v>
+      </c>
+      <c r="J49">
+        <v>100</v>
+      </c>
+      <c r="K49" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50">
+        <v>5</v>
+      </c>
+      <c r="C50">
+        <v>158</v>
+      </c>
+      <c r="D50" t="str">
+        <f t="shared" si="1"/>
+        <v>\cite{RefWorks:5}</v>
+      </c>
+      <c r="G50">
+        <v>5</v>
+      </c>
+      <c r="J50">
+        <v>105</v>
+      </c>
+      <c r="K50" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51">
+        <v>60</v>
+      </c>
+      <c r="C51">
+        <v>96</v>
+      </c>
+      <c r="D51" t="str">
+        <f t="shared" si="1"/>
+        <v>\cite{RefWorks:60}</v>
+      </c>
+      <c r="G51">
+        <v>60</v>
+      </c>
+      <c r="J51">
+        <v>108</v>
+      </c>
+      <c r="K51">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52">
+        <v>218</v>
+      </c>
+      <c r="C52">
+        <v>35</v>
+      </c>
+      <c r="D52" t="str">
+        <f t="shared" si="1"/>
+        <v>\cite{RefWorks:218}</v>
+      </c>
+      <c r="G52">
+        <v>218</v>
+      </c>
+      <c r="J52">
+        <v>109</v>
+      </c>
+      <c r="K52">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53">
+        <v>65</v>
+      </c>
+      <c r="C53">
+        <v>46</v>
+      </c>
+      <c r="D53" t="str">
+        <f t="shared" si="1"/>
+        <v>\cite{RefWorks:65}</v>
+      </c>
+      <c r="G53">
+        <v>65</v>
+      </c>
+      <c r="J53">
+        <v>110</v>
+      </c>
+      <c r="K53">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54">
+        <v>505</v>
+      </c>
+      <c r="D54" t="str">
+        <f t="shared" si="1"/>
+        <v>\cite{RefWorks:505}</v>
+      </c>
+      <c r="G54">
+        <v>505</v>
+      </c>
+      <c r="J54">
+        <v>111</v>
+      </c>
+      <c r="K54">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55">
+        <v>386</v>
+      </c>
+      <c r="D55" t="str">
+        <f t="shared" si="1"/>
+        <v>\cite{RefWorks:386}</v>
+      </c>
+      <c r="G55">
+        <v>386</v>
+      </c>
+      <c r="J55">
+        <v>116</v>
+      </c>
+      <c r="K55">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G56">
         <v>0</v>
+      </c>
+      <c r="J56">
+        <v>117</v>
+      </c>
+      <c r="K56">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J57">
+        <v>129</v>
+      </c>
+      <c r="K57">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J58">
+        <v>143</v>
+      </c>
+      <c r="K58" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J59">
+        <v>156</v>
+      </c>
+      <c r="K59" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J60">
+        <v>167</v>
+      </c>
+      <c r="K60">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J61">
+        <v>169</v>
+      </c>
+      <c r="K61" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J62">
+        <v>170</v>
+      </c>
+      <c r="K62" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J63">
+        <v>171</v>
+      </c>
+      <c r="K63">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J64">
+        <v>172</v>
+      </c>
+      <c r="K64">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B500">
     <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
-      <formula>AND(COUNTIF($E$2:$E$100,B2)=1,(INDEX($A$2:$A$500,MATCH(B2,$B$2:$B$500,0)))&lt;&gt;A2)</formula>
+      <formula>AND(COUNTIF($G$2:$G$100,B2)=1,(INDEX($A$2:$A$500,MATCH(B2,$B$2:$B$500,0)))&lt;&gt;A2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2">
+  <conditionalFormatting sqref="K2">
     <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
-      <formula>I2="Reference Not Used Yet!"</formula>
+      <formula>K2="Reference Not Used Yet!"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -5792,14 +6588,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="40c2d214-4ca5-4604-be72-e6c4439e5276">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="581c75f3-c23e-4d61-ac2d-458e1df0a137" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6016,27 +6810,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="40c2d214-4ca5-4604-be72-e6c4439e5276">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="581c75f3-c23e-4d61-ac2d-458e1df0a137" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F17E70AE-5CD9-46AD-9CD7-253B7D5337F5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77CBFA7D-3A0A-48A4-8B12-895234E5D6E5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="40c2d214-4ca5-4604-be72-e6c4439e5276"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="581c75f3-c23e-4d61-ac2d-458e1df0a137"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6061,9 +6848,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77CBFA7D-3A0A-48A4-8B12-895234E5D6E5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F17E70AE-5CD9-46AD-9CD7-253B7D5337F5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="581c75f3-c23e-4d61-ac2d-458e1df0a137"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="40c2d214-4ca5-4604-be72-e6c4439e5276"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>